<commit_message>
fix npe; add an experimental feature
</commit_message>
<xml_diff>
--- a/data/2021战绩_1.xlsx
+++ b/data/2021战绩_1.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86471\IdeaProjects\divide-squad\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2325FC9A-DE39-4BA6-B260-6444905C896F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70407D2F-5A98-49E7-B12B-A884AC0BE033}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23040" windowHeight="12204" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="2021-05-29-分队方案" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$29</definedName>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="69">
   <si>
     <r>
       <rPr>
@@ -514,6 +516,63 @@
     <t>丙</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>方案一</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>总能力值</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力均值</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A队</t>
+  </si>
+  <si>
+    <t>A队</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>B队</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>孙</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>方</t>
+    </r>
+  </si>
+  <si>
+    <t>方案二</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -522,7 +581,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -567,6 +626,19 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -588,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -616,6 +688,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,7 +1021,7 @@
   <dimension ref="A1:AMK29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1921,7 +2008,7 @@
   <dimension ref="A1:AMK30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="A1:F30"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2540,15 +2627,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969451C8-386D-4A08-AE84-4C7B11DFC183}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:1025">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -2568,7 +2655,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:1025">
       <c r="A2" s="9" t="s">
         <v>18</v>
       </c>
@@ -2588,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:1025">
       <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
@@ -2608,7 +2695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:1025">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -2628,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:1025">
       <c r="A5" s="3" t="s">
         <v>39</v>
       </c>
@@ -2648,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:1025">
       <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
@@ -2668,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:1025">
       <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
@@ -2688,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:1025">
       <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
@@ -2708,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:1025">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -2728,7 +2815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:1025">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -2748,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:1025">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -2768,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:1025">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
@@ -2788,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:1025">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -2808,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:1025" ht="13.8" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -2828,8 +2915,4259 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="E15" s="3"/>
+    <row r="15" spans="1:1025" ht="13.2" customHeight="1">
+      <c r="A15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="1"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="1"/>
+      <c r="BJ15" s="1"/>
+      <c r="BK15" s="1"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+      <c r="BO15" s="1"/>
+      <c r="BP15" s="1"/>
+      <c r="BQ15" s="1"/>
+      <c r="BR15" s="1"/>
+      <c r="BS15" s="1"/>
+      <c r="BT15" s="1"/>
+      <c r="BU15" s="1"/>
+      <c r="BV15" s="1"/>
+      <c r="BW15" s="1"/>
+      <c r="BX15" s="1"/>
+      <c r="BY15" s="1"/>
+      <c r="BZ15" s="1"/>
+      <c r="CA15" s="1"/>
+      <c r="CB15" s="1"/>
+      <c r="CC15" s="1"/>
+      <c r="CD15" s="1"/>
+      <c r="CE15" s="1"/>
+      <c r="CF15" s="1"/>
+      <c r="CG15" s="1"/>
+      <c r="CH15" s="1"/>
+      <c r="CI15" s="1"/>
+      <c r="CJ15" s="1"/>
+      <c r="CK15" s="1"/>
+      <c r="CL15" s="1"/>
+      <c r="CM15" s="1"/>
+      <c r="CN15" s="1"/>
+      <c r="CO15" s="1"/>
+      <c r="CP15" s="1"/>
+      <c r="CQ15" s="1"/>
+      <c r="CR15" s="1"/>
+      <c r="CS15" s="1"/>
+      <c r="CT15" s="1"/>
+      <c r="CU15" s="1"/>
+      <c r="CV15" s="1"/>
+      <c r="CW15" s="1"/>
+      <c r="CX15" s="1"/>
+      <c r="CY15" s="1"/>
+      <c r="CZ15" s="1"/>
+      <c r="DA15" s="1"/>
+      <c r="DB15" s="1"/>
+      <c r="DC15" s="1"/>
+      <c r="DD15" s="1"/>
+      <c r="DE15" s="1"/>
+      <c r="DF15" s="1"/>
+      <c r="DG15" s="1"/>
+      <c r="DH15" s="1"/>
+      <c r="DI15" s="1"/>
+      <c r="DJ15" s="1"/>
+      <c r="DK15" s="1"/>
+      <c r="DL15" s="1"/>
+      <c r="DM15" s="1"/>
+      <c r="DN15" s="1"/>
+      <c r="DO15" s="1"/>
+      <c r="DP15" s="1"/>
+      <c r="DQ15" s="1"/>
+      <c r="DR15" s="1"/>
+      <c r="DS15" s="1"/>
+      <c r="DT15" s="1"/>
+      <c r="DU15" s="1"/>
+      <c r="DV15" s="1"/>
+      <c r="DW15" s="1"/>
+      <c r="DX15" s="1"/>
+      <c r="DY15" s="1"/>
+      <c r="DZ15" s="1"/>
+      <c r="EA15" s="1"/>
+      <c r="EB15" s="1"/>
+      <c r="EC15" s="1"/>
+      <c r="ED15" s="1"/>
+      <c r="EE15" s="1"/>
+      <c r="EF15" s="1"/>
+      <c r="EG15" s="1"/>
+      <c r="EH15" s="1"/>
+      <c r="EI15" s="1"/>
+      <c r="EJ15" s="1"/>
+      <c r="EK15" s="1"/>
+      <c r="EL15" s="1"/>
+      <c r="EM15" s="1"/>
+      <c r="EN15" s="1"/>
+      <c r="EO15" s="1"/>
+      <c r="EP15" s="1"/>
+      <c r="EQ15" s="1"/>
+      <c r="ER15" s="1"/>
+      <c r="ES15" s="1"/>
+      <c r="ET15" s="1"/>
+      <c r="EU15" s="1"/>
+      <c r="EV15" s="1"/>
+      <c r="EW15" s="1"/>
+      <c r="EX15" s="1"/>
+      <c r="EY15" s="1"/>
+      <c r="EZ15" s="1"/>
+      <c r="FA15" s="1"/>
+      <c r="FB15" s="1"/>
+      <c r="FC15" s="1"/>
+      <c r="FD15" s="1"/>
+      <c r="FE15" s="1"/>
+      <c r="FF15" s="1"/>
+      <c r="FG15" s="1"/>
+      <c r="FH15" s="1"/>
+      <c r="FI15" s="1"/>
+      <c r="FJ15" s="1"/>
+      <c r="FK15" s="1"/>
+      <c r="FL15" s="1"/>
+      <c r="FM15" s="1"/>
+      <c r="FN15" s="1"/>
+      <c r="FO15" s="1"/>
+      <c r="FP15" s="1"/>
+      <c r="FQ15" s="1"/>
+      <c r="FR15" s="1"/>
+      <c r="FS15" s="1"/>
+      <c r="FT15" s="1"/>
+      <c r="FU15" s="1"/>
+      <c r="FV15" s="1"/>
+      <c r="FW15" s="1"/>
+      <c r="FX15" s="1"/>
+      <c r="FY15" s="1"/>
+      <c r="FZ15" s="1"/>
+      <c r="GA15" s="1"/>
+      <c r="GB15" s="1"/>
+      <c r="GC15" s="1"/>
+      <c r="GD15" s="1"/>
+      <c r="GE15" s="1"/>
+      <c r="GF15" s="1"/>
+      <c r="GG15" s="1"/>
+      <c r="GH15" s="1"/>
+      <c r="GI15" s="1"/>
+      <c r="GJ15" s="1"/>
+      <c r="GK15" s="1"/>
+      <c r="GL15" s="1"/>
+      <c r="GM15" s="1"/>
+      <c r="GN15" s="1"/>
+      <c r="GO15" s="1"/>
+      <c r="GP15" s="1"/>
+      <c r="GQ15" s="1"/>
+      <c r="GR15" s="1"/>
+      <c r="GS15" s="1"/>
+      <c r="GT15" s="1"/>
+      <c r="GU15" s="1"/>
+      <c r="GV15" s="1"/>
+      <c r="GW15" s="1"/>
+      <c r="GX15" s="1"/>
+      <c r="GY15" s="1"/>
+      <c r="GZ15" s="1"/>
+      <c r="HA15" s="1"/>
+      <c r="HB15" s="1"/>
+      <c r="HC15" s="1"/>
+      <c r="HD15" s="1"/>
+      <c r="HE15" s="1"/>
+      <c r="HF15" s="1"/>
+      <c r="HG15" s="1"/>
+      <c r="HH15" s="1"/>
+      <c r="HI15" s="1"/>
+      <c r="HJ15" s="1"/>
+      <c r="HK15" s="1"/>
+      <c r="HL15" s="1"/>
+      <c r="HM15" s="1"/>
+      <c r="HN15" s="1"/>
+      <c r="HO15" s="1"/>
+      <c r="HP15" s="1"/>
+      <c r="HQ15" s="1"/>
+      <c r="HR15" s="1"/>
+      <c r="HS15" s="1"/>
+      <c r="HT15" s="1"/>
+      <c r="HU15" s="1"/>
+      <c r="HV15" s="1"/>
+      <c r="HW15" s="1"/>
+      <c r="HX15" s="1"/>
+      <c r="HY15" s="1"/>
+      <c r="HZ15" s="1"/>
+      <c r="IA15" s="1"/>
+      <c r="IB15" s="1"/>
+      <c r="IC15" s="1"/>
+      <c r="ID15" s="1"/>
+      <c r="IE15" s="1"/>
+      <c r="IF15" s="1"/>
+      <c r="IG15" s="1"/>
+      <c r="IH15" s="1"/>
+      <c r="II15" s="1"/>
+      <c r="IJ15" s="1"/>
+      <c r="IK15" s="1"/>
+      <c r="IL15" s="1"/>
+      <c r="IM15" s="1"/>
+      <c r="IN15" s="1"/>
+      <c r="IO15" s="1"/>
+      <c r="IP15" s="1"/>
+      <c r="IQ15" s="1"/>
+      <c r="IR15" s="1"/>
+      <c r="IS15" s="1"/>
+      <c r="IT15" s="1"/>
+      <c r="IU15" s="1"/>
+      <c r="IV15" s="1"/>
+      <c r="IW15" s="1"/>
+      <c r="IX15" s="1"/>
+      <c r="IY15" s="1"/>
+      <c r="IZ15" s="1"/>
+      <c r="JA15" s="1"/>
+      <c r="JB15" s="1"/>
+      <c r="JC15" s="1"/>
+      <c r="JD15" s="1"/>
+      <c r="JE15" s="1"/>
+      <c r="JF15" s="1"/>
+      <c r="JG15" s="1"/>
+      <c r="JH15" s="1"/>
+      <c r="JI15" s="1"/>
+      <c r="JJ15" s="1"/>
+      <c r="JK15" s="1"/>
+      <c r="JL15" s="1"/>
+      <c r="JM15" s="1"/>
+      <c r="JN15" s="1"/>
+      <c r="JO15" s="1"/>
+      <c r="JP15" s="1"/>
+      <c r="JQ15" s="1"/>
+      <c r="JR15" s="1"/>
+      <c r="JS15" s="1"/>
+      <c r="JT15" s="1"/>
+      <c r="JU15" s="1"/>
+      <c r="JV15" s="1"/>
+      <c r="JW15" s="1"/>
+      <c r="JX15" s="1"/>
+      <c r="JY15" s="1"/>
+      <c r="JZ15" s="1"/>
+      <c r="KA15" s="1"/>
+      <c r="KB15" s="1"/>
+      <c r="KC15" s="1"/>
+      <c r="KD15" s="1"/>
+      <c r="KE15" s="1"/>
+      <c r="KF15" s="1"/>
+      <c r="KG15" s="1"/>
+      <c r="KH15" s="1"/>
+      <c r="KI15" s="1"/>
+      <c r="KJ15" s="1"/>
+      <c r="KK15" s="1"/>
+      <c r="KL15" s="1"/>
+      <c r="KM15" s="1"/>
+      <c r="KN15" s="1"/>
+      <c r="KO15" s="1"/>
+      <c r="KP15" s="1"/>
+      <c r="KQ15" s="1"/>
+      <c r="KR15" s="1"/>
+      <c r="KS15" s="1"/>
+      <c r="KT15" s="1"/>
+      <c r="KU15" s="1"/>
+      <c r="KV15" s="1"/>
+      <c r="KW15" s="1"/>
+      <c r="KX15" s="1"/>
+      <c r="KY15" s="1"/>
+      <c r="KZ15" s="1"/>
+      <c r="LA15" s="1"/>
+      <c r="LB15" s="1"/>
+      <c r="LC15" s="1"/>
+      <c r="LD15" s="1"/>
+      <c r="LE15" s="1"/>
+      <c r="LF15" s="1"/>
+      <c r="LG15" s="1"/>
+      <c r="LH15" s="1"/>
+      <c r="LI15" s="1"/>
+      <c r="LJ15" s="1"/>
+      <c r="LK15" s="1"/>
+      <c r="LL15" s="1"/>
+      <c r="LM15" s="1"/>
+      <c r="LN15" s="1"/>
+      <c r="LO15" s="1"/>
+      <c r="LP15" s="1"/>
+      <c r="LQ15" s="1"/>
+      <c r="LR15" s="1"/>
+      <c r="LS15" s="1"/>
+      <c r="LT15" s="1"/>
+      <c r="LU15" s="1"/>
+      <c r="LV15" s="1"/>
+      <c r="LW15" s="1"/>
+      <c r="LX15" s="1"/>
+      <c r="LY15" s="1"/>
+      <c r="LZ15" s="1"/>
+      <c r="MA15" s="1"/>
+      <c r="MB15" s="1"/>
+      <c r="MC15" s="1"/>
+      <c r="MD15" s="1"/>
+      <c r="ME15" s="1"/>
+      <c r="MF15" s="1"/>
+      <c r="MG15" s="1"/>
+      <c r="MH15" s="1"/>
+      <c r="MI15" s="1"/>
+      <c r="MJ15" s="1"/>
+      <c r="MK15" s="1"/>
+      <c r="ML15" s="1"/>
+      <c r="MM15" s="1"/>
+      <c r="MN15" s="1"/>
+      <c r="MO15" s="1"/>
+      <c r="MP15" s="1"/>
+      <c r="MQ15" s="1"/>
+      <c r="MR15" s="1"/>
+      <c r="MS15" s="1"/>
+      <c r="MT15" s="1"/>
+      <c r="MU15" s="1"/>
+      <c r="MV15" s="1"/>
+      <c r="MW15" s="1"/>
+      <c r="MX15" s="1"/>
+      <c r="MY15" s="1"/>
+      <c r="MZ15" s="1"/>
+      <c r="NA15" s="1"/>
+      <c r="NB15" s="1"/>
+      <c r="NC15" s="1"/>
+      <c r="ND15" s="1"/>
+      <c r="NE15" s="1"/>
+      <c r="NF15" s="1"/>
+      <c r="NG15" s="1"/>
+      <c r="NH15" s="1"/>
+      <c r="NI15" s="1"/>
+      <c r="NJ15" s="1"/>
+      <c r="NK15" s="1"/>
+      <c r="NL15" s="1"/>
+      <c r="NM15" s="1"/>
+      <c r="NN15" s="1"/>
+      <c r="NO15" s="1"/>
+      <c r="NP15" s="1"/>
+      <c r="NQ15" s="1"/>
+      <c r="NR15" s="1"/>
+      <c r="NS15" s="1"/>
+      <c r="NT15" s="1"/>
+      <c r="NU15" s="1"/>
+      <c r="NV15" s="1"/>
+      <c r="NW15" s="1"/>
+      <c r="NX15" s="1"/>
+      <c r="NY15" s="1"/>
+      <c r="NZ15" s="1"/>
+      <c r="OA15" s="1"/>
+      <c r="OB15" s="1"/>
+      <c r="OC15" s="1"/>
+      <c r="OD15" s="1"/>
+      <c r="OE15" s="1"/>
+      <c r="OF15" s="1"/>
+      <c r="OG15" s="1"/>
+      <c r="OH15" s="1"/>
+      <c r="OI15" s="1"/>
+      <c r="OJ15" s="1"/>
+      <c r="OK15" s="1"/>
+      <c r="OL15" s="1"/>
+      <c r="OM15" s="1"/>
+      <c r="ON15" s="1"/>
+      <c r="OO15" s="1"/>
+      <c r="OP15" s="1"/>
+      <c r="OQ15" s="1"/>
+      <c r="OR15" s="1"/>
+      <c r="OS15" s="1"/>
+      <c r="OT15" s="1"/>
+      <c r="OU15" s="1"/>
+      <c r="OV15" s="1"/>
+      <c r="OW15" s="1"/>
+      <c r="OX15" s="1"/>
+      <c r="OY15" s="1"/>
+      <c r="OZ15" s="1"/>
+      <c r="PA15" s="1"/>
+      <c r="PB15" s="1"/>
+      <c r="PC15" s="1"/>
+      <c r="PD15" s="1"/>
+      <c r="PE15" s="1"/>
+      <c r="PF15" s="1"/>
+      <c r="PG15" s="1"/>
+      <c r="PH15" s="1"/>
+      <c r="PI15" s="1"/>
+      <c r="PJ15" s="1"/>
+      <c r="PK15" s="1"/>
+      <c r="PL15" s="1"/>
+      <c r="PM15" s="1"/>
+      <c r="PN15" s="1"/>
+      <c r="PO15" s="1"/>
+      <c r="PP15" s="1"/>
+      <c r="PQ15" s="1"/>
+      <c r="PR15" s="1"/>
+      <c r="PS15" s="1"/>
+      <c r="PT15" s="1"/>
+      <c r="PU15" s="1"/>
+      <c r="PV15" s="1"/>
+      <c r="PW15" s="1"/>
+      <c r="PX15" s="1"/>
+      <c r="PY15" s="1"/>
+      <c r="PZ15" s="1"/>
+      <c r="QA15" s="1"/>
+      <c r="QB15" s="1"/>
+      <c r="QC15" s="1"/>
+      <c r="QD15" s="1"/>
+      <c r="QE15" s="1"/>
+      <c r="QF15" s="1"/>
+      <c r="QG15" s="1"/>
+      <c r="QH15" s="1"/>
+      <c r="QI15" s="1"/>
+      <c r="QJ15" s="1"/>
+      <c r="QK15" s="1"/>
+      <c r="QL15" s="1"/>
+      <c r="QM15" s="1"/>
+      <c r="QN15" s="1"/>
+      <c r="QO15" s="1"/>
+      <c r="QP15" s="1"/>
+      <c r="QQ15" s="1"/>
+      <c r="QR15" s="1"/>
+      <c r="QS15" s="1"/>
+      <c r="QT15" s="1"/>
+      <c r="QU15" s="1"/>
+      <c r="QV15" s="1"/>
+      <c r="QW15" s="1"/>
+      <c r="QX15" s="1"/>
+      <c r="QY15" s="1"/>
+      <c r="QZ15" s="1"/>
+      <c r="RA15" s="1"/>
+      <c r="RB15" s="1"/>
+      <c r="RC15" s="1"/>
+      <c r="RD15" s="1"/>
+      <c r="RE15" s="1"/>
+      <c r="RF15" s="1"/>
+      <c r="RG15" s="1"/>
+      <c r="RH15" s="1"/>
+      <c r="RI15" s="1"/>
+      <c r="RJ15" s="1"/>
+      <c r="RK15" s="1"/>
+      <c r="RL15" s="1"/>
+      <c r="RM15" s="1"/>
+      <c r="RN15" s="1"/>
+      <c r="RO15" s="1"/>
+      <c r="RP15" s="1"/>
+      <c r="RQ15" s="1"/>
+      <c r="RR15" s="1"/>
+      <c r="RS15" s="1"/>
+      <c r="RT15" s="1"/>
+      <c r="RU15" s="1"/>
+      <c r="RV15" s="1"/>
+      <c r="RW15" s="1"/>
+      <c r="RX15" s="1"/>
+      <c r="RY15" s="1"/>
+      <c r="RZ15" s="1"/>
+      <c r="SA15" s="1"/>
+      <c r="SB15" s="1"/>
+      <c r="SC15" s="1"/>
+      <c r="SD15" s="1"/>
+      <c r="SE15" s="1"/>
+      <c r="SF15" s="1"/>
+      <c r="SG15" s="1"/>
+      <c r="SH15" s="1"/>
+      <c r="SI15" s="1"/>
+      <c r="SJ15" s="1"/>
+      <c r="SK15" s="1"/>
+      <c r="SL15" s="1"/>
+      <c r="SM15" s="1"/>
+      <c r="SN15" s="1"/>
+      <c r="SO15" s="1"/>
+      <c r="SP15" s="1"/>
+      <c r="SQ15" s="1"/>
+      <c r="SR15" s="1"/>
+      <c r="SS15" s="1"/>
+      <c r="ST15" s="1"/>
+      <c r="SU15" s="1"/>
+      <c r="SV15" s="1"/>
+      <c r="SW15" s="1"/>
+      <c r="SX15" s="1"/>
+      <c r="SY15" s="1"/>
+      <c r="SZ15" s="1"/>
+      <c r="TA15" s="1"/>
+      <c r="TB15" s="1"/>
+      <c r="TC15" s="1"/>
+      <c r="TD15" s="1"/>
+      <c r="TE15" s="1"/>
+      <c r="TF15" s="1"/>
+      <c r="TG15" s="1"/>
+      <c r="TH15" s="1"/>
+      <c r="TI15" s="1"/>
+      <c r="TJ15" s="1"/>
+      <c r="TK15" s="1"/>
+      <c r="TL15" s="1"/>
+      <c r="TM15" s="1"/>
+      <c r="TN15" s="1"/>
+      <c r="TO15" s="1"/>
+      <c r="TP15" s="1"/>
+      <c r="TQ15" s="1"/>
+      <c r="TR15" s="1"/>
+      <c r="TS15" s="1"/>
+      <c r="TT15" s="1"/>
+      <c r="TU15" s="1"/>
+      <c r="TV15" s="1"/>
+      <c r="TW15" s="1"/>
+      <c r="TX15" s="1"/>
+      <c r="TY15" s="1"/>
+      <c r="TZ15" s="1"/>
+      <c r="UA15" s="1"/>
+      <c r="UB15" s="1"/>
+      <c r="UC15" s="1"/>
+      <c r="UD15" s="1"/>
+      <c r="UE15" s="1"/>
+      <c r="UF15" s="1"/>
+      <c r="UG15" s="1"/>
+      <c r="UH15" s="1"/>
+      <c r="UI15" s="1"/>
+      <c r="UJ15" s="1"/>
+      <c r="UK15" s="1"/>
+      <c r="UL15" s="1"/>
+      <c r="UM15" s="1"/>
+      <c r="UN15" s="1"/>
+      <c r="UO15" s="1"/>
+      <c r="UP15" s="1"/>
+      <c r="UQ15" s="1"/>
+      <c r="UR15" s="1"/>
+      <c r="US15" s="1"/>
+      <c r="UT15" s="1"/>
+      <c r="UU15" s="1"/>
+      <c r="UV15" s="1"/>
+      <c r="UW15" s="1"/>
+      <c r="UX15" s="1"/>
+      <c r="UY15" s="1"/>
+      <c r="UZ15" s="1"/>
+      <c r="VA15" s="1"/>
+      <c r="VB15" s="1"/>
+      <c r="VC15" s="1"/>
+      <c r="VD15" s="1"/>
+      <c r="VE15" s="1"/>
+      <c r="VF15" s="1"/>
+      <c r="VG15" s="1"/>
+      <c r="VH15" s="1"/>
+      <c r="VI15" s="1"/>
+      <c r="VJ15" s="1"/>
+      <c r="VK15" s="1"/>
+      <c r="VL15" s="1"/>
+      <c r="VM15" s="1"/>
+      <c r="VN15" s="1"/>
+      <c r="VO15" s="1"/>
+      <c r="VP15" s="1"/>
+      <c r="VQ15" s="1"/>
+      <c r="VR15" s="1"/>
+      <c r="VS15" s="1"/>
+      <c r="VT15" s="1"/>
+      <c r="VU15" s="1"/>
+      <c r="VV15" s="1"/>
+      <c r="VW15" s="1"/>
+      <c r="VX15" s="1"/>
+      <c r="VY15" s="1"/>
+      <c r="VZ15" s="1"/>
+      <c r="WA15" s="1"/>
+      <c r="WB15" s="1"/>
+      <c r="WC15" s="1"/>
+      <c r="WD15" s="1"/>
+      <c r="WE15" s="1"/>
+      <c r="WF15" s="1"/>
+      <c r="WG15" s="1"/>
+      <c r="WH15" s="1"/>
+      <c r="WI15" s="1"/>
+      <c r="WJ15" s="1"/>
+      <c r="WK15" s="1"/>
+      <c r="WL15" s="1"/>
+      <c r="WM15" s="1"/>
+      <c r="WN15" s="1"/>
+      <c r="WO15" s="1"/>
+      <c r="WP15" s="1"/>
+      <c r="WQ15" s="1"/>
+      <c r="WR15" s="1"/>
+      <c r="WS15" s="1"/>
+      <c r="WT15" s="1"/>
+      <c r="WU15" s="1"/>
+      <c r="WV15" s="1"/>
+      <c r="WW15" s="1"/>
+      <c r="WX15" s="1"/>
+      <c r="WY15" s="1"/>
+      <c r="WZ15" s="1"/>
+      <c r="XA15" s="1"/>
+      <c r="XB15" s="1"/>
+      <c r="XC15" s="1"/>
+      <c r="XD15" s="1"/>
+      <c r="XE15" s="1"/>
+      <c r="XF15" s="1"/>
+      <c r="XG15" s="1"/>
+      <c r="XH15" s="1"/>
+      <c r="XI15" s="1"/>
+      <c r="XJ15" s="1"/>
+      <c r="XK15" s="1"/>
+      <c r="XL15" s="1"/>
+      <c r="XM15" s="1"/>
+      <c r="XN15" s="1"/>
+      <c r="XO15" s="1"/>
+      <c r="XP15" s="1"/>
+      <c r="XQ15" s="1"/>
+      <c r="XR15" s="1"/>
+      <c r="XS15" s="1"/>
+      <c r="XT15" s="1"/>
+      <c r="XU15" s="1"/>
+      <c r="XV15" s="1"/>
+      <c r="XW15" s="1"/>
+      <c r="XX15" s="1"/>
+      <c r="XY15" s="1"/>
+      <c r="XZ15" s="1"/>
+      <c r="YA15" s="1"/>
+      <c r="YB15" s="1"/>
+      <c r="YC15" s="1"/>
+      <c r="YD15" s="1"/>
+      <c r="YE15" s="1"/>
+      <c r="YF15" s="1"/>
+      <c r="YG15" s="1"/>
+      <c r="YH15" s="1"/>
+      <c r="YI15" s="1"/>
+      <c r="YJ15" s="1"/>
+      <c r="YK15" s="1"/>
+      <c r="YL15" s="1"/>
+      <c r="YM15" s="1"/>
+      <c r="YN15" s="1"/>
+      <c r="YO15" s="1"/>
+      <c r="YP15" s="1"/>
+      <c r="YQ15" s="1"/>
+      <c r="YR15" s="1"/>
+      <c r="YS15" s="1"/>
+      <c r="YT15" s="1"/>
+      <c r="YU15" s="1"/>
+      <c r="YV15" s="1"/>
+      <c r="YW15" s="1"/>
+      <c r="YX15" s="1"/>
+      <c r="YY15" s="1"/>
+      <c r="YZ15" s="1"/>
+      <c r="ZA15" s="1"/>
+      <c r="ZB15" s="1"/>
+      <c r="ZC15" s="1"/>
+      <c r="ZD15" s="1"/>
+      <c r="ZE15" s="1"/>
+      <c r="ZF15" s="1"/>
+      <c r="ZG15" s="1"/>
+      <c r="ZH15" s="1"/>
+      <c r="ZI15" s="1"/>
+      <c r="ZJ15" s="1"/>
+      <c r="ZK15" s="1"/>
+      <c r="ZL15" s="1"/>
+      <c r="ZM15" s="1"/>
+      <c r="ZN15" s="1"/>
+      <c r="ZO15" s="1"/>
+      <c r="ZP15" s="1"/>
+      <c r="ZQ15" s="1"/>
+      <c r="ZR15" s="1"/>
+      <c r="ZS15" s="1"/>
+      <c r="ZT15" s="1"/>
+      <c r="ZU15" s="1"/>
+      <c r="ZV15" s="1"/>
+      <c r="ZW15" s="1"/>
+      <c r="ZX15" s="1"/>
+      <c r="ZY15" s="1"/>
+      <c r="ZZ15" s="1"/>
+      <c r="AAA15" s="1"/>
+      <c r="AAB15" s="1"/>
+      <c r="AAC15" s="1"/>
+      <c r="AAD15" s="1"/>
+      <c r="AAE15" s="1"/>
+      <c r="AAF15" s="1"/>
+      <c r="AAG15" s="1"/>
+      <c r="AAH15" s="1"/>
+      <c r="AAI15" s="1"/>
+      <c r="AAJ15" s="1"/>
+      <c r="AAK15" s="1"/>
+      <c r="AAL15" s="1"/>
+      <c r="AAM15" s="1"/>
+      <c r="AAN15" s="1"/>
+      <c r="AAO15" s="1"/>
+      <c r="AAP15" s="1"/>
+      <c r="AAQ15" s="1"/>
+      <c r="AAR15" s="1"/>
+      <c r="AAS15" s="1"/>
+      <c r="AAT15" s="1"/>
+      <c r="AAU15" s="1"/>
+      <c r="AAV15" s="1"/>
+      <c r="AAW15" s="1"/>
+      <c r="AAX15" s="1"/>
+      <c r="AAY15" s="1"/>
+      <c r="AAZ15" s="1"/>
+      <c r="ABA15" s="1"/>
+      <c r="ABB15" s="1"/>
+      <c r="ABC15" s="1"/>
+      <c r="ABD15" s="1"/>
+      <c r="ABE15" s="1"/>
+      <c r="ABF15" s="1"/>
+      <c r="ABG15" s="1"/>
+      <c r="ABH15" s="1"/>
+      <c r="ABI15" s="1"/>
+      <c r="ABJ15" s="1"/>
+      <c r="ABK15" s="1"/>
+      <c r="ABL15" s="1"/>
+      <c r="ABM15" s="1"/>
+      <c r="ABN15" s="1"/>
+      <c r="ABO15" s="1"/>
+      <c r="ABP15" s="1"/>
+      <c r="ABQ15" s="1"/>
+      <c r="ABR15" s="1"/>
+      <c r="ABS15" s="1"/>
+      <c r="ABT15" s="1"/>
+      <c r="ABU15" s="1"/>
+      <c r="ABV15" s="1"/>
+      <c r="ABW15" s="1"/>
+      <c r="ABX15" s="1"/>
+      <c r="ABY15" s="1"/>
+      <c r="ABZ15" s="1"/>
+      <c r="ACA15" s="1"/>
+      <c r="ACB15" s="1"/>
+      <c r="ACC15" s="1"/>
+      <c r="ACD15" s="1"/>
+      <c r="ACE15" s="1"/>
+      <c r="ACF15" s="1"/>
+      <c r="ACG15" s="1"/>
+      <c r="ACH15" s="1"/>
+      <c r="ACI15" s="1"/>
+      <c r="ACJ15" s="1"/>
+      <c r="ACK15" s="1"/>
+      <c r="ACL15" s="1"/>
+      <c r="ACM15" s="1"/>
+      <c r="ACN15" s="1"/>
+      <c r="ACO15" s="1"/>
+      <c r="ACP15" s="1"/>
+      <c r="ACQ15" s="1"/>
+      <c r="ACR15" s="1"/>
+      <c r="ACS15" s="1"/>
+      <c r="ACT15" s="1"/>
+      <c r="ACU15" s="1"/>
+      <c r="ACV15" s="1"/>
+      <c r="ACW15" s="1"/>
+      <c r="ACX15" s="1"/>
+      <c r="ACY15" s="1"/>
+      <c r="ACZ15" s="1"/>
+      <c r="ADA15" s="1"/>
+      <c r="ADB15" s="1"/>
+      <c r="ADC15" s="1"/>
+      <c r="ADD15" s="1"/>
+      <c r="ADE15" s="1"/>
+      <c r="ADF15" s="1"/>
+      <c r="ADG15" s="1"/>
+      <c r="ADH15" s="1"/>
+      <c r="ADI15" s="1"/>
+      <c r="ADJ15" s="1"/>
+      <c r="ADK15" s="1"/>
+      <c r="ADL15" s="1"/>
+      <c r="ADM15" s="1"/>
+      <c r="ADN15" s="1"/>
+      <c r="ADO15" s="1"/>
+      <c r="ADP15" s="1"/>
+      <c r="ADQ15" s="1"/>
+      <c r="ADR15" s="1"/>
+      <c r="ADS15" s="1"/>
+      <c r="ADT15" s="1"/>
+      <c r="ADU15" s="1"/>
+      <c r="ADV15" s="1"/>
+      <c r="ADW15" s="1"/>
+      <c r="ADX15" s="1"/>
+      <c r="ADY15" s="1"/>
+      <c r="ADZ15" s="1"/>
+      <c r="AEA15" s="1"/>
+      <c r="AEB15" s="1"/>
+      <c r="AEC15" s="1"/>
+      <c r="AED15" s="1"/>
+      <c r="AEE15" s="1"/>
+      <c r="AEF15" s="1"/>
+      <c r="AEG15" s="1"/>
+      <c r="AEH15" s="1"/>
+      <c r="AEI15" s="1"/>
+      <c r="AEJ15" s="1"/>
+      <c r="AEK15" s="1"/>
+      <c r="AEL15" s="1"/>
+      <c r="AEM15" s="1"/>
+      <c r="AEN15" s="1"/>
+      <c r="AEO15" s="1"/>
+      <c r="AEP15" s="1"/>
+      <c r="AEQ15" s="1"/>
+      <c r="AER15" s="1"/>
+      <c r="AES15" s="1"/>
+      <c r="AET15" s="1"/>
+      <c r="AEU15" s="1"/>
+      <c r="AEV15" s="1"/>
+      <c r="AEW15" s="1"/>
+      <c r="AEX15" s="1"/>
+      <c r="AEY15" s="1"/>
+      <c r="AEZ15" s="1"/>
+      <c r="AFA15" s="1"/>
+      <c r="AFB15" s="1"/>
+      <c r="AFC15" s="1"/>
+      <c r="AFD15" s="1"/>
+      <c r="AFE15" s="1"/>
+      <c r="AFF15" s="1"/>
+      <c r="AFG15" s="1"/>
+      <c r="AFH15" s="1"/>
+      <c r="AFI15" s="1"/>
+      <c r="AFJ15" s="1"/>
+      <c r="AFK15" s="1"/>
+      <c r="AFL15" s="1"/>
+      <c r="AFM15" s="1"/>
+      <c r="AFN15" s="1"/>
+      <c r="AFO15" s="1"/>
+      <c r="AFP15" s="1"/>
+      <c r="AFQ15" s="1"/>
+      <c r="AFR15" s="1"/>
+      <c r="AFS15" s="1"/>
+      <c r="AFT15" s="1"/>
+      <c r="AFU15" s="1"/>
+      <c r="AFV15" s="1"/>
+      <c r="AFW15" s="1"/>
+      <c r="AFX15" s="1"/>
+      <c r="AFY15" s="1"/>
+      <c r="AFZ15" s="1"/>
+      <c r="AGA15" s="1"/>
+      <c r="AGB15" s="1"/>
+      <c r="AGC15" s="1"/>
+      <c r="AGD15" s="1"/>
+      <c r="AGE15" s="1"/>
+      <c r="AGF15" s="1"/>
+      <c r="AGG15" s="1"/>
+      <c r="AGH15" s="1"/>
+      <c r="AGI15" s="1"/>
+      <c r="AGJ15" s="1"/>
+      <c r="AGK15" s="1"/>
+      <c r="AGL15" s="1"/>
+      <c r="AGM15" s="1"/>
+      <c r="AGN15" s="1"/>
+      <c r="AGO15" s="1"/>
+      <c r="AGP15" s="1"/>
+      <c r="AGQ15" s="1"/>
+      <c r="AGR15" s="1"/>
+      <c r="AGS15" s="1"/>
+      <c r="AGT15" s="1"/>
+      <c r="AGU15" s="1"/>
+      <c r="AGV15" s="1"/>
+      <c r="AGW15" s="1"/>
+      <c r="AGX15" s="1"/>
+      <c r="AGY15" s="1"/>
+      <c r="AGZ15" s="1"/>
+      <c r="AHA15" s="1"/>
+      <c r="AHB15" s="1"/>
+      <c r="AHC15" s="1"/>
+      <c r="AHD15" s="1"/>
+      <c r="AHE15" s="1"/>
+      <c r="AHF15" s="1"/>
+      <c r="AHG15" s="1"/>
+      <c r="AHH15" s="1"/>
+      <c r="AHI15" s="1"/>
+      <c r="AHJ15" s="1"/>
+      <c r="AHK15" s="1"/>
+      <c r="AHL15" s="1"/>
+      <c r="AHM15" s="1"/>
+      <c r="AHN15" s="1"/>
+      <c r="AHO15" s="1"/>
+      <c r="AHP15" s="1"/>
+      <c r="AHQ15" s="1"/>
+      <c r="AHR15" s="1"/>
+      <c r="AHS15" s="1"/>
+      <c r="AHT15" s="1"/>
+      <c r="AHU15" s="1"/>
+      <c r="AHV15" s="1"/>
+      <c r="AHW15" s="1"/>
+      <c r="AHX15" s="1"/>
+      <c r="AHY15" s="1"/>
+      <c r="AHZ15" s="1"/>
+      <c r="AIA15" s="1"/>
+      <c r="AIB15" s="1"/>
+      <c r="AIC15" s="1"/>
+      <c r="AID15" s="1"/>
+      <c r="AIE15" s="1"/>
+      <c r="AIF15" s="1"/>
+      <c r="AIG15" s="1"/>
+      <c r="AIH15" s="1"/>
+      <c r="AII15" s="1"/>
+      <c r="AIJ15" s="1"/>
+      <c r="AIK15" s="1"/>
+      <c r="AIL15" s="1"/>
+      <c r="AIM15" s="1"/>
+      <c r="AIN15" s="1"/>
+      <c r="AIO15" s="1"/>
+      <c r="AIP15" s="1"/>
+      <c r="AIQ15" s="1"/>
+      <c r="AIR15" s="1"/>
+      <c r="AIS15" s="1"/>
+      <c r="AIT15" s="1"/>
+      <c r="AIU15" s="1"/>
+      <c r="AIV15" s="1"/>
+      <c r="AIW15" s="1"/>
+      <c r="AIX15" s="1"/>
+      <c r="AIY15" s="1"/>
+      <c r="AIZ15" s="1"/>
+      <c r="AJA15" s="1"/>
+      <c r="AJB15" s="1"/>
+      <c r="AJC15" s="1"/>
+      <c r="AJD15" s="1"/>
+      <c r="AJE15" s="1"/>
+      <c r="AJF15" s="1"/>
+      <c r="AJG15" s="1"/>
+      <c r="AJH15" s="1"/>
+      <c r="AJI15" s="1"/>
+      <c r="AJJ15" s="1"/>
+      <c r="AJK15" s="1"/>
+      <c r="AJL15" s="1"/>
+      <c r="AJM15" s="1"/>
+      <c r="AJN15" s="1"/>
+      <c r="AJO15" s="1"/>
+      <c r="AJP15" s="1"/>
+      <c r="AJQ15" s="1"/>
+      <c r="AJR15" s="1"/>
+      <c r="AJS15" s="1"/>
+      <c r="AJT15" s="1"/>
+      <c r="AJU15" s="1"/>
+      <c r="AJV15" s="1"/>
+      <c r="AJW15" s="1"/>
+      <c r="AJX15" s="1"/>
+      <c r="AJY15" s="1"/>
+      <c r="AJZ15" s="1"/>
+      <c r="AKA15" s="1"/>
+      <c r="AKB15" s="1"/>
+      <c r="AKC15" s="1"/>
+      <c r="AKD15" s="1"/>
+      <c r="AKE15" s="1"/>
+      <c r="AKF15" s="1"/>
+      <c r="AKG15" s="1"/>
+      <c r="AKH15" s="1"/>
+      <c r="AKI15" s="1"/>
+      <c r="AKJ15" s="1"/>
+      <c r="AKK15" s="1"/>
+      <c r="AKL15" s="1"/>
+      <c r="AKM15" s="1"/>
+      <c r="AKN15" s="1"/>
+      <c r="AKO15" s="1"/>
+      <c r="AKP15" s="1"/>
+      <c r="AKQ15" s="1"/>
+      <c r="AKR15" s="1"/>
+      <c r="AKS15" s="1"/>
+      <c r="AKT15" s="1"/>
+      <c r="AKU15" s="1"/>
+      <c r="AKV15" s="1"/>
+      <c r="AKW15" s="1"/>
+      <c r="AKX15" s="1"/>
+      <c r="AKY15" s="1"/>
+      <c r="AKZ15" s="1"/>
+      <c r="ALA15" s="1"/>
+      <c r="ALB15" s="1"/>
+      <c r="ALC15" s="1"/>
+      <c r="ALD15" s="1"/>
+      <c r="ALE15" s="1"/>
+      <c r="ALF15" s="1"/>
+      <c r="ALG15" s="1"/>
+      <c r="ALH15" s="1"/>
+      <c r="ALI15" s="1"/>
+      <c r="ALJ15" s="1"/>
+      <c r="ALK15" s="1"/>
+      <c r="ALL15" s="1"/>
+      <c r="ALM15" s="1"/>
+      <c r="ALN15" s="1"/>
+      <c r="ALO15" s="1"/>
+      <c r="ALP15" s="1"/>
+      <c r="ALQ15" s="1"/>
+      <c r="ALR15" s="1"/>
+      <c r="ALS15" s="1"/>
+      <c r="ALT15" s="1"/>
+      <c r="ALU15" s="1"/>
+      <c r="ALV15" s="1"/>
+      <c r="ALW15" s="1"/>
+      <c r="ALX15" s="1"/>
+      <c r="ALY15" s="1"/>
+      <c r="ALZ15" s="1"/>
+      <c r="AMA15" s="1"/>
+      <c r="AMB15" s="1"/>
+      <c r="AMC15" s="1"/>
+      <c r="AMD15" s="1"/>
+      <c r="AME15" s="1"/>
+      <c r="AMF15" s="1"/>
+      <c r="AMG15" s="1"/>
+      <c r="AMH15" s="1"/>
+      <c r="AMI15" s="1"/>
+      <c r="AMJ15" s="1"/>
+      <c r="AMK15" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAA2729-4AA7-45F0-B3EE-D6FC7C744A86}">
+  <dimension ref="A1:AMK34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1025">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1025">
+      <c r="A2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1025">
+      <c r="A3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1025">
+      <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1025">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1025">
+      <c r="A6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1025">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1025">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1025">
+      <c r="A9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1025">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1025">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1025">
+      <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1025">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1025">
+      <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1025" ht="13.2" customHeight="1">
+      <c r="A15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="1"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="1"/>
+      <c r="BJ15" s="1"/>
+      <c r="BK15" s="1"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+      <c r="BO15" s="1"/>
+      <c r="BP15" s="1"/>
+      <c r="BQ15" s="1"/>
+      <c r="BR15" s="1"/>
+      <c r="BS15" s="1"/>
+      <c r="BT15" s="1"/>
+      <c r="BU15" s="1"/>
+      <c r="BV15" s="1"/>
+      <c r="BW15" s="1"/>
+      <c r="BX15" s="1"/>
+      <c r="BY15" s="1"/>
+      <c r="BZ15" s="1"/>
+      <c r="CA15" s="1"/>
+      <c r="CB15" s="1"/>
+      <c r="CC15" s="1"/>
+      <c r="CD15" s="1"/>
+      <c r="CE15" s="1"/>
+      <c r="CF15" s="1"/>
+      <c r="CG15" s="1"/>
+      <c r="CH15" s="1"/>
+      <c r="CI15" s="1"/>
+      <c r="CJ15" s="1"/>
+      <c r="CK15" s="1"/>
+      <c r="CL15" s="1"/>
+      <c r="CM15" s="1"/>
+      <c r="CN15" s="1"/>
+      <c r="CO15" s="1"/>
+      <c r="CP15" s="1"/>
+      <c r="CQ15" s="1"/>
+      <c r="CR15" s="1"/>
+      <c r="CS15" s="1"/>
+      <c r="CT15" s="1"/>
+      <c r="CU15" s="1"/>
+      <c r="CV15" s="1"/>
+      <c r="CW15" s="1"/>
+      <c r="CX15" s="1"/>
+      <c r="CY15" s="1"/>
+      <c r="CZ15" s="1"/>
+      <c r="DA15" s="1"/>
+      <c r="DB15" s="1"/>
+      <c r="DC15" s="1"/>
+      <c r="DD15" s="1"/>
+      <c r="DE15" s="1"/>
+      <c r="DF15" s="1"/>
+      <c r="DG15" s="1"/>
+      <c r="DH15" s="1"/>
+      <c r="DI15" s="1"/>
+      <c r="DJ15" s="1"/>
+      <c r="DK15" s="1"/>
+      <c r="DL15" s="1"/>
+      <c r="DM15" s="1"/>
+      <c r="DN15" s="1"/>
+      <c r="DO15" s="1"/>
+      <c r="DP15" s="1"/>
+      <c r="DQ15" s="1"/>
+      <c r="DR15" s="1"/>
+      <c r="DS15" s="1"/>
+      <c r="DT15" s="1"/>
+      <c r="DU15" s="1"/>
+      <c r="DV15" s="1"/>
+      <c r="DW15" s="1"/>
+      <c r="DX15" s="1"/>
+      <c r="DY15" s="1"/>
+      <c r="DZ15" s="1"/>
+      <c r="EA15" s="1"/>
+      <c r="EB15" s="1"/>
+      <c r="EC15" s="1"/>
+      <c r="ED15" s="1"/>
+      <c r="EE15" s="1"/>
+      <c r="EF15" s="1"/>
+      <c r="EG15" s="1"/>
+      <c r="EH15" s="1"/>
+      <c r="EI15" s="1"/>
+      <c r="EJ15" s="1"/>
+      <c r="EK15" s="1"/>
+      <c r="EL15" s="1"/>
+      <c r="EM15" s="1"/>
+      <c r="EN15" s="1"/>
+      <c r="EO15" s="1"/>
+      <c r="EP15" s="1"/>
+      <c r="EQ15" s="1"/>
+      <c r="ER15" s="1"/>
+      <c r="ES15" s="1"/>
+      <c r="ET15" s="1"/>
+      <c r="EU15" s="1"/>
+      <c r="EV15" s="1"/>
+      <c r="EW15" s="1"/>
+      <c r="EX15" s="1"/>
+      <c r="EY15" s="1"/>
+      <c r="EZ15" s="1"/>
+      <c r="FA15" s="1"/>
+      <c r="FB15" s="1"/>
+      <c r="FC15" s="1"/>
+      <c r="FD15" s="1"/>
+      <c r="FE15" s="1"/>
+      <c r="FF15" s="1"/>
+      <c r="FG15" s="1"/>
+      <c r="FH15" s="1"/>
+      <c r="FI15" s="1"/>
+      <c r="FJ15" s="1"/>
+      <c r="FK15" s="1"/>
+      <c r="FL15" s="1"/>
+      <c r="FM15" s="1"/>
+      <c r="FN15" s="1"/>
+      <c r="FO15" s="1"/>
+      <c r="FP15" s="1"/>
+      <c r="FQ15" s="1"/>
+      <c r="FR15" s="1"/>
+      <c r="FS15" s="1"/>
+      <c r="FT15" s="1"/>
+      <c r="FU15" s="1"/>
+      <c r="FV15" s="1"/>
+      <c r="FW15" s="1"/>
+      <c r="FX15" s="1"/>
+      <c r="FY15" s="1"/>
+      <c r="FZ15" s="1"/>
+      <c r="GA15" s="1"/>
+      <c r="GB15" s="1"/>
+      <c r="GC15" s="1"/>
+      <c r="GD15" s="1"/>
+      <c r="GE15" s="1"/>
+      <c r="GF15" s="1"/>
+      <c r="GG15" s="1"/>
+      <c r="GH15" s="1"/>
+      <c r="GI15" s="1"/>
+      <c r="GJ15" s="1"/>
+      <c r="GK15" s="1"/>
+      <c r="GL15" s="1"/>
+      <c r="GM15" s="1"/>
+      <c r="GN15" s="1"/>
+      <c r="GO15" s="1"/>
+      <c r="GP15" s="1"/>
+      <c r="GQ15" s="1"/>
+      <c r="GR15" s="1"/>
+      <c r="GS15" s="1"/>
+      <c r="GT15" s="1"/>
+      <c r="GU15" s="1"/>
+      <c r="GV15" s="1"/>
+      <c r="GW15" s="1"/>
+      <c r="GX15" s="1"/>
+      <c r="GY15" s="1"/>
+      <c r="GZ15" s="1"/>
+      <c r="HA15" s="1"/>
+      <c r="HB15" s="1"/>
+      <c r="HC15" s="1"/>
+      <c r="HD15" s="1"/>
+      <c r="HE15" s="1"/>
+      <c r="HF15" s="1"/>
+      <c r="HG15" s="1"/>
+      <c r="HH15" s="1"/>
+      <c r="HI15" s="1"/>
+      <c r="HJ15" s="1"/>
+      <c r="HK15" s="1"/>
+      <c r="HL15" s="1"/>
+      <c r="HM15" s="1"/>
+      <c r="HN15" s="1"/>
+      <c r="HO15" s="1"/>
+      <c r="HP15" s="1"/>
+      <c r="HQ15" s="1"/>
+      <c r="HR15" s="1"/>
+      <c r="HS15" s="1"/>
+      <c r="HT15" s="1"/>
+      <c r="HU15" s="1"/>
+      <c r="HV15" s="1"/>
+      <c r="HW15" s="1"/>
+      <c r="HX15" s="1"/>
+      <c r="HY15" s="1"/>
+      <c r="HZ15" s="1"/>
+      <c r="IA15" s="1"/>
+      <c r="IB15" s="1"/>
+      <c r="IC15" s="1"/>
+      <c r="ID15" s="1"/>
+      <c r="IE15" s="1"/>
+      <c r="IF15" s="1"/>
+      <c r="IG15" s="1"/>
+      <c r="IH15" s="1"/>
+      <c r="II15" s="1"/>
+      <c r="IJ15" s="1"/>
+      <c r="IK15" s="1"/>
+      <c r="IL15" s="1"/>
+      <c r="IM15" s="1"/>
+      <c r="IN15" s="1"/>
+      <c r="IO15" s="1"/>
+      <c r="IP15" s="1"/>
+      <c r="IQ15" s="1"/>
+      <c r="IR15" s="1"/>
+      <c r="IS15" s="1"/>
+      <c r="IT15" s="1"/>
+      <c r="IU15" s="1"/>
+      <c r="IV15" s="1"/>
+      <c r="IW15" s="1"/>
+      <c r="IX15" s="1"/>
+      <c r="IY15" s="1"/>
+      <c r="IZ15" s="1"/>
+      <c r="JA15" s="1"/>
+      <c r="JB15" s="1"/>
+      <c r="JC15" s="1"/>
+      <c r="JD15" s="1"/>
+      <c r="JE15" s="1"/>
+      <c r="JF15" s="1"/>
+      <c r="JG15" s="1"/>
+      <c r="JH15" s="1"/>
+      <c r="JI15" s="1"/>
+      <c r="JJ15" s="1"/>
+      <c r="JK15" s="1"/>
+      <c r="JL15" s="1"/>
+      <c r="JM15" s="1"/>
+      <c r="JN15" s="1"/>
+      <c r="JO15" s="1"/>
+      <c r="JP15" s="1"/>
+      <c r="JQ15" s="1"/>
+      <c r="JR15" s="1"/>
+      <c r="JS15" s="1"/>
+      <c r="JT15" s="1"/>
+      <c r="JU15" s="1"/>
+      <c r="JV15" s="1"/>
+      <c r="JW15" s="1"/>
+      <c r="JX15" s="1"/>
+      <c r="JY15" s="1"/>
+      <c r="JZ15" s="1"/>
+      <c r="KA15" s="1"/>
+      <c r="KB15" s="1"/>
+      <c r="KC15" s="1"/>
+      <c r="KD15" s="1"/>
+      <c r="KE15" s="1"/>
+      <c r="KF15" s="1"/>
+      <c r="KG15" s="1"/>
+      <c r="KH15" s="1"/>
+      <c r="KI15" s="1"/>
+      <c r="KJ15" s="1"/>
+      <c r="KK15" s="1"/>
+      <c r="KL15" s="1"/>
+      <c r="KM15" s="1"/>
+      <c r="KN15" s="1"/>
+      <c r="KO15" s="1"/>
+      <c r="KP15" s="1"/>
+      <c r="KQ15" s="1"/>
+      <c r="KR15" s="1"/>
+      <c r="KS15" s="1"/>
+      <c r="KT15" s="1"/>
+      <c r="KU15" s="1"/>
+      <c r="KV15" s="1"/>
+      <c r="KW15" s="1"/>
+      <c r="KX15" s="1"/>
+      <c r="KY15" s="1"/>
+      <c r="KZ15" s="1"/>
+      <c r="LA15" s="1"/>
+      <c r="LB15" s="1"/>
+      <c r="LC15" s="1"/>
+      <c r="LD15" s="1"/>
+      <c r="LE15" s="1"/>
+      <c r="LF15" s="1"/>
+      <c r="LG15" s="1"/>
+      <c r="LH15" s="1"/>
+      <c r="LI15" s="1"/>
+      <c r="LJ15" s="1"/>
+      <c r="LK15" s="1"/>
+      <c r="LL15" s="1"/>
+      <c r="LM15" s="1"/>
+      <c r="LN15" s="1"/>
+      <c r="LO15" s="1"/>
+      <c r="LP15" s="1"/>
+      <c r="LQ15" s="1"/>
+      <c r="LR15" s="1"/>
+      <c r="LS15" s="1"/>
+      <c r="LT15" s="1"/>
+      <c r="LU15" s="1"/>
+      <c r="LV15" s="1"/>
+      <c r="LW15" s="1"/>
+      <c r="LX15" s="1"/>
+      <c r="LY15" s="1"/>
+      <c r="LZ15" s="1"/>
+      <c r="MA15" s="1"/>
+      <c r="MB15" s="1"/>
+      <c r="MC15" s="1"/>
+      <c r="MD15" s="1"/>
+      <c r="ME15" s="1"/>
+      <c r="MF15" s="1"/>
+      <c r="MG15" s="1"/>
+      <c r="MH15" s="1"/>
+      <c r="MI15" s="1"/>
+      <c r="MJ15" s="1"/>
+      <c r="MK15" s="1"/>
+      <c r="ML15" s="1"/>
+      <c r="MM15" s="1"/>
+      <c r="MN15" s="1"/>
+      <c r="MO15" s="1"/>
+      <c r="MP15" s="1"/>
+      <c r="MQ15" s="1"/>
+      <c r="MR15" s="1"/>
+      <c r="MS15" s="1"/>
+      <c r="MT15" s="1"/>
+      <c r="MU15" s="1"/>
+      <c r="MV15" s="1"/>
+      <c r="MW15" s="1"/>
+      <c r="MX15" s="1"/>
+      <c r="MY15" s="1"/>
+      <c r="MZ15" s="1"/>
+      <c r="NA15" s="1"/>
+      <c r="NB15" s="1"/>
+      <c r="NC15" s="1"/>
+      <c r="ND15" s="1"/>
+      <c r="NE15" s="1"/>
+      <c r="NF15" s="1"/>
+      <c r="NG15" s="1"/>
+      <c r="NH15" s="1"/>
+      <c r="NI15" s="1"/>
+      <c r="NJ15" s="1"/>
+      <c r="NK15" s="1"/>
+      <c r="NL15" s="1"/>
+      <c r="NM15" s="1"/>
+      <c r="NN15" s="1"/>
+      <c r="NO15" s="1"/>
+      <c r="NP15" s="1"/>
+      <c r="NQ15" s="1"/>
+      <c r="NR15" s="1"/>
+      <c r="NS15" s="1"/>
+      <c r="NT15" s="1"/>
+      <c r="NU15" s="1"/>
+      <c r="NV15" s="1"/>
+      <c r="NW15" s="1"/>
+      <c r="NX15" s="1"/>
+      <c r="NY15" s="1"/>
+      <c r="NZ15" s="1"/>
+      <c r="OA15" s="1"/>
+      <c r="OB15" s="1"/>
+      <c r="OC15" s="1"/>
+      <c r="OD15" s="1"/>
+      <c r="OE15" s="1"/>
+      <c r="OF15" s="1"/>
+      <c r="OG15" s="1"/>
+      <c r="OH15" s="1"/>
+      <c r="OI15" s="1"/>
+      <c r="OJ15" s="1"/>
+      <c r="OK15" s="1"/>
+      <c r="OL15" s="1"/>
+      <c r="OM15" s="1"/>
+      <c r="ON15" s="1"/>
+      <c r="OO15" s="1"/>
+      <c r="OP15" s="1"/>
+      <c r="OQ15" s="1"/>
+      <c r="OR15" s="1"/>
+      <c r="OS15" s="1"/>
+      <c r="OT15" s="1"/>
+      <c r="OU15" s="1"/>
+      <c r="OV15" s="1"/>
+      <c r="OW15" s="1"/>
+      <c r="OX15" s="1"/>
+      <c r="OY15" s="1"/>
+      <c r="OZ15" s="1"/>
+      <c r="PA15" s="1"/>
+      <c r="PB15" s="1"/>
+      <c r="PC15" s="1"/>
+      <c r="PD15" s="1"/>
+      <c r="PE15" s="1"/>
+      <c r="PF15" s="1"/>
+      <c r="PG15" s="1"/>
+      <c r="PH15" s="1"/>
+      <c r="PI15" s="1"/>
+      <c r="PJ15" s="1"/>
+      <c r="PK15" s="1"/>
+      <c r="PL15" s="1"/>
+      <c r="PM15" s="1"/>
+      <c r="PN15" s="1"/>
+      <c r="PO15" s="1"/>
+      <c r="PP15" s="1"/>
+      <c r="PQ15" s="1"/>
+      <c r="PR15" s="1"/>
+      <c r="PS15" s="1"/>
+      <c r="PT15" s="1"/>
+      <c r="PU15" s="1"/>
+      <c r="PV15" s="1"/>
+      <c r="PW15" s="1"/>
+      <c r="PX15" s="1"/>
+      <c r="PY15" s="1"/>
+      <c r="PZ15" s="1"/>
+      <c r="QA15" s="1"/>
+      <c r="QB15" s="1"/>
+      <c r="QC15" s="1"/>
+      <c r="QD15" s="1"/>
+      <c r="QE15" s="1"/>
+      <c r="QF15" s="1"/>
+      <c r="QG15" s="1"/>
+      <c r="QH15" s="1"/>
+      <c r="QI15" s="1"/>
+      <c r="QJ15" s="1"/>
+      <c r="QK15" s="1"/>
+      <c r="QL15" s="1"/>
+      <c r="QM15" s="1"/>
+      <c r="QN15" s="1"/>
+      <c r="QO15" s="1"/>
+      <c r="QP15" s="1"/>
+      <c r="QQ15" s="1"/>
+      <c r="QR15" s="1"/>
+      <c r="QS15" s="1"/>
+      <c r="QT15" s="1"/>
+      <c r="QU15" s="1"/>
+      <c r="QV15" s="1"/>
+      <c r="QW15" s="1"/>
+      <c r="QX15" s="1"/>
+      <c r="QY15" s="1"/>
+      <c r="QZ15" s="1"/>
+      <c r="RA15" s="1"/>
+      <c r="RB15" s="1"/>
+      <c r="RC15" s="1"/>
+      <c r="RD15" s="1"/>
+      <c r="RE15" s="1"/>
+      <c r="RF15" s="1"/>
+      <c r="RG15" s="1"/>
+      <c r="RH15" s="1"/>
+      <c r="RI15" s="1"/>
+      <c r="RJ15" s="1"/>
+      <c r="RK15" s="1"/>
+      <c r="RL15" s="1"/>
+      <c r="RM15" s="1"/>
+      <c r="RN15" s="1"/>
+      <c r="RO15" s="1"/>
+      <c r="RP15" s="1"/>
+      <c r="RQ15" s="1"/>
+      <c r="RR15" s="1"/>
+      <c r="RS15" s="1"/>
+      <c r="RT15" s="1"/>
+      <c r="RU15" s="1"/>
+      <c r="RV15" s="1"/>
+      <c r="RW15" s="1"/>
+      <c r="RX15" s="1"/>
+      <c r="RY15" s="1"/>
+      <c r="RZ15" s="1"/>
+      <c r="SA15" s="1"/>
+      <c r="SB15" s="1"/>
+      <c r="SC15" s="1"/>
+      <c r="SD15" s="1"/>
+      <c r="SE15" s="1"/>
+      <c r="SF15" s="1"/>
+      <c r="SG15" s="1"/>
+      <c r="SH15" s="1"/>
+      <c r="SI15" s="1"/>
+      <c r="SJ15" s="1"/>
+      <c r="SK15" s="1"/>
+      <c r="SL15" s="1"/>
+      <c r="SM15" s="1"/>
+      <c r="SN15" s="1"/>
+      <c r="SO15" s="1"/>
+      <c r="SP15" s="1"/>
+      <c r="SQ15" s="1"/>
+      <c r="SR15" s="1"/>
+      <c r="SS15" s="1"/>
+      <c r="ST15" s="1"/>
+      <c r="SU15" s="1"/>
+      <c r="SV15" s="1"/>
+      <c r="SW15" s="1"/>
+      <c r="SX15" s="1"/>
+      <c r="SY15" s="1"/>
+      <c r="SZ15" s="1"/>
+      <c r="TA15" s="1"/>
+      <c r="TB15" s="1"/>
+      <c r="TC15" s="1"/>
+      <c r="TD15" s="1"/>
+      <c r="TE15" s="1"/>
+      <c r="TF15" s="1"/>
+      <c r="TG15" s="1"/>
+      <c r="TH15" s="1"/>
+      <c r="TI15" s="1"/>
+      <c r="TJ15" s="1"/>
+      <c r="TK15" s="1"/>
+      <c r="TL15" s="1"/>
+      <c r="TM15" s="1"/>
+      <c r="TN15" s="1"/>
+      <c r="TO15" s="1"/>
+      <c r="TP15" s="1"/>
+      <c r="TQ15" s="1"/>
+      <c r="TR15" s="1"/>
+      <c r="TS15" s="1"/>
+      <c r="TT15" s="1"/>
+      <c r="TU15" s="1"/>
+      <c r="TV15" s="1"/>
+      <c r="TW15" s="1"/>
+      <c r="TX15" s="1"/>
+      <c r="TY15" s="1"/>
+      <c r="TZ15" s="1"/>
+      <c r="UA15" s="1"/>
+      <c r="UB15" s="1"/>
+      <c r="UC15" s="1"/>
+      <c r="UD15" s="1"/>
+      <c r="UE15" s="1"/>
+      <c r="UF15" s="1"/>
+      <c r="UG15" s="1"/>
+      <c r="UH15" s="1"/>
+      <c r="UI15" s="1"/>
+      <c r="UJ15" s="1"/>
+      <c r="UK15" s="1"/>
+      <c r="UL15" s="1"/>
+      <c r="UM15" s="1"/>
+      <c r="UN15" s="1"/>
+      <c r="UO15" s="1"/>
+      <c r="UP15" s="1"/>
+      <c r="UQ15" s="1"/>
+      <c r="UR15" s="1"/>
+      <c r="US15" s="1"/>
+      <c r="UT15" s="1"/>
+      <c r="UU15" s="1"/>
+      <c r="UV15" s="1"/>
+      <c r="UW15" s="1"/>
+      <c r="UX15" s="1"/>
+      <c r="UY15" s="1"/>
+      <c r="UZ15" s="1"/>
+      <c r="VA15" s="1"/>
+      <c r="VB15" s="1"/>
+      <c r="VC15" s="1"/>
+      <c r="VD15" s="1"/>
+      <c r="VE15" s="1"/>
+      <c r="VF15" s="1"/>
+      <c r="VG15" s="1"/>
+      <c r="VH15" s="1"/>
+      <c r="VI15" s="1"/>
+      <c r="VJ15" s="1"/>
+      <c r="VK15" s="1"/>
+      <c r="VL15" s="1"/>
+      <c r="VM15" s="1"/>
+      <c r="VN15" s="1"/>
+      <c r="VO15" s="1"/>
+      <c r="VP15" s="1"/>
+      <c r="VQ15" s="1"/>
+      <c r="VR15" s="1"/>
+      <c r="VS15" s="1"/>
+      <c r="VT15" s="1"/>
+      <c r="VU15" s="1"/>
+      <c r="VV15" s="1"/>
+      <c r="VW15" s="1"/>
+      <c r="VX15" s="1"/>
+      <c r="VY15" s="1"/>
+      <c r="VZ15" s="1"/>
+      <c r="WA15" s="1"/>
+      <c r="WB15" s="1"/>
+      <c r="WC15" s="1"/>
+      <c r="WD15" s="1"/>
+      <c r="WE15" s="1"/>
+      <c r="WF15" s="1"/>
+      <c r="WG15" s="1"/>
+      <c r="WH15" s="1"/>
+      <c r="WI15" s="1"/>
+      <c r="WJ15" s="1"/>
+      <c r="WK15" s="1"/>
+      <c r="WL15" s="1"/>
+      <c r="WM15" s="1"/>
+      <c r="WN15" s="1"/>
+      <c r="WO15" s="1"/>
+      <c r="WP15" s="1"/>
+      <c r="WQ15" s="1"/>
+      <c r="WR15" s="1"/>
+      <c r="WS15" s="1"/>
+      <c r="WT15" s="1"/>
+      <c r="WU15" s="1"/>
+      <c r="WV15" s="1"/>
+      <c r="WW15" s="1"/>
+      <c r="WX15" s="1"/>
+      <c r="WY15" s="1"/>
+      <c r="WZ15" s="1"/>
+      <c r="XA15" s="1"/>
+      <c r="XB15" s="1"/>
+      <c r="XC15" s="1"/>
+      <c r="XD15" s="1"/>
+      <c r="XE15" s="1"/>
+      <c r="XF15" s="1"/>
+      <c r="XG15" s="1"/>
+      <c r="XH15" s="1"/>
+      <c r="XI15" s="1"/>
+      <c r="XJ15" s="1"/>
+      <c r="XK15" s="1"/>
+      <c r="XL15" s="1"/>
+      <c r="XM15" s="1"/>
+      <c r="XN15" s="1"/>
+      <c r="XO15" s="1"/>
+      <c r="XP15" s="1"/>
+      <c r="XQ15" s="1"/>
+      <c r="XR15" s="1"/>
+      <c r="XS15" s="1"/>
+      <c r="XT15" s="1"/>
+      <c r="XU15" s="1"/>
+      <c r="XV15" s="1"/>
+      <c r="XW15" s="1"/>
+      <c r="XX15" s="1"/>
+      <c r="XY15" s="1"/>
+      <c r="XZ15" s="1"/>
+      <c r="YA15" s="1"/>
+      <c r="YB15" s="1"/>
+      <c r="YC15" s="1"/>
+      <c r="YD15" s="1"/>
+      <c r="YE15" s="1"/>
+      <c r="YF15" s="1"/>
+      <c r="YG15" s="1"/>
+      <c r="YH15" s="1"/>
+      <c r="YI15" s="1"/>
+      <c r="YJ15" s="1"/>
+      <c r="YK15" s="1"/>
+      <c r="YL15" s="1"/>
+      <c r="YM15" s="1"/>
+      <c r="YN15" s="1"/>
+      <c r="YO15" s="1"/>
+      <c r="YP15" s="1"/>
+      <c r="YQ15" s="1"/>
+      <c r="YR15" s="1"/>
+      <c r="YS15" s="1"/>
+      <c r="YT15" s="1"/>
+      <c r="YU15" s="1"/>
+      <c r="YV15" s="1"/>
+      <c r="YW15" s="1"/>
+      <c r="YX15" s="1"/>
+      <c r="YY15" s="1"/>
+      <c r="YZ15" s="1"/>
+      <c r="ZA15" s="1"/>
+      <c r="ZB15" s="1"/>
+      <c r="ZC15" s="1"/>
+      <c r="ZD15" s="1"/>
+      <c r="ZE15" s="1"/>
+      <c r="ZF15" s="1"/>
+      <c r="ZG15" s="1"/>
+      <c r="ZH15" s="1"/>
+      <c r="ZI15" s="1"/>
+      <c r="ZJ15" s="1"/>
+      <c r="ZK15" s="1"/>
+      <c r="ZL15" s="1"/>
+      <c r="ZM15" s="1"/>
+      <c r="ZN15" s="1"/>
+      <c r="ZO15" s="1"/>
+      <c r="ZP15" s="1"/>
+      <c r="ZQ15" s="1"/>
+      <c r="ZR15" s="1"/>
+      <c r="ZS15" s="1"/>
+      <c r="ZT15" s="1"/>
+      <c r="ZU15" s="1"/>
+      <c r="ZV15" s="1"/>
+      <c r="ZW15" s="1"/>
+      <c r="ZX15" s="1"/>
+      <c r="ZY15" s="1"/>
+      <c r="ZZ15" s="1"/>
+      <c r="AAA15" s="1"/>
+      <c r="AAB15" s="1"/>
+      <c r="AAC15" s="1"/>
+      <c r="AAD15" s="1"/>
+      <c r="AAE15" s="1"/>
+      <c r="AAF15" s="1"/>
+      <c r="AAG15" s="1"/>
+      <c r="AAH15" s="1"/>
+      <c r="AAI15" s="1"/>
+      <c r="AAJ15" s="1"/>
+      <c r="AAK15" s="1"/>
+      <c r="AAL15" s="1"/>
+      <c r="AAM15" s="1"/>
+      <c r="AAN15" s="1"/>
+      <c r="AAO15" s="1"/>
+      <c r="AAP15" s="1"/>
+      <c r="AAQ15" s="1"/>
+      <c r="AAR15" s="1"/>
+      <c r="AAS15" s="1"/>
+      <c r="AAT15" s="1"/>
+      <c r="AAU15" s="1"/>
+      <c r="AAV15" s="1"/>
+      <c r="AAW15" s="1"/>
+      <c r="AAX15" s="1"/>
+      <c r="AAY15" s="1"/>
+      <c r="AAZ15" s="1"/>
+      <c r="ABA15" s="1"/>
+      <c r="ABB15" s="1"/>
+      <c r="ABC15" s="1"/>
+      <c r="ABD15" s="1"/>
+      <c r="ABE15" s="1"/>
+      <c r="ABF15" s="1"/>
+      <c r="ABG15" s="1"/>
+      <c r="ABH15" s="1"/>
+      <c r="ABI15" s="1"/>
+      <c r="ABJ15" s="1"/>
+      <c r="ABK15" s="1"/>
+      <c r="ABL15" s="1"/>
+      <c r="ABM15" s="1"/>
+      <c r="ABN15" s="1"/>
+      <c r="ABO15" s="1"/>
+      <c r="ABP15" s="1"/>
+      <c r="ABQ15" s="1"/>
+      <c r="ABR15" s="1"/>
+      <c r="ABS15" s="1"/>
+      <c r="ABT15" s="1"/>
+      <c r="ABU15" s="1"/>
+      <c r="ABV15" s="1"/>
+      <c r="ABW15" s="1"/>
+      <c r="ABX15" s="1"/>
+      <c r="ABY15" s="1"/>
+      <c r="ABZ15" s="1"/>
+      <c r="ACA15" s="1"/>
+      <c r="ACB15" s="1"/>
+      <c r="ACC15" s="1"/>
+      <c r="ACD15" s="1"/>
+      <c r="ACE15" s="1"/>
+      <c r="ACF15" s="1"/>
+      <c r="ACG15" s="1"/>
+      <c r="ACH15" s="1"/>
+      <c r="ACI15" s="1"/>
+      <c r="ACJ15" s="1"/>
+      <c r="ACK15" s="1"/>
+      <c r="ACL15" s="1"/>
+      <c r="ACM15" s="1"/>
+      <c r="ACN15" s="1"/>
+      <c r="ACO15" s="1"/>
+      <c r="ACP15" s="1"/>
+      <c r="ACQ15" s="1"/>
+      <c r="ACR15" s="1"/>
+      <c r="ACS15" s="1"/>
+      <c r="ACT15" s="1"/>
+      <c r="ACU15" s="1"/>
+      <c r="ACV15" s="1"/>
+      <c r="ACW15" s="1"/>
+      <c r="ACX15" s="1"/>
+      <c r="ACY15" s="1"/>
+      <c r="ACZ15" s="1"/>
+      <c r="ADA15" s="1"/>
+      <c r="ADB15" s="1"/>
+      <c r="ADC15" s="1"/>
+      <c r="ADD15" s="1"/>
+      <c r="ADE15" s="1"/>
+      <c r="ADF15" s="1"/>
+      <c r="ADG15" s="1"/>
+      <c r="ADH15" s="1"/>
+      <c r="ADI15" s="1"/>
+      <c r="ADJ15" s="1"/>
+      <c r="ADK15" s="1"/>
+      <c r="ADL15" s="1"/>
+      <c r="ADM15" s="1"/>
+      <c r="ADN15" s="1"/>
+      <c r="ADO15" s="1"/>
+      <c r="ADP15" s="1"/>
+      <c r="ADQ15" s="1"/>
+      <c r="ADR15" s="1"/>
+      <c r="ADS15" s="1"/>
+      <c r="ADT15" s="1"/>
+      <c r="ADU15" s="1"/>
+      <c r="ADV15" s="1"/>
+      <c r="ADW15" s="1"/>
+      <c r="ADX15" s="1"/>
+      <c r="ADY15" s="1"/>
+      <c r="ADZ15" s="1"/>
+      <c r="AEA15" s="1"/>
+      <c r="AEB15" s="1"/>
+      <c r="AEC15" s="1"/>
+      <c r="AED15" s="1"/>
+      <c r="AEE15" s="1"/>
+      <c r="AEF15" s="1"/>
+      <c r="AEG15" s="1"/>
+      <c r="AEH15" s="1"/>
+      <c r="AEI15" s="1"/>
+      <c r="AEJ15" s="1"/>
+      <c r="AEK15" s="1"/>
+      <c r="AEL15" s="1"/>
+      <c r="AEM15" s="1"/>
+      <c r="AEN15" s="1"/>
+      <c r="AEO15" s="1"/>
+      <c r="AEP15" s="1"/>
+      <c r="AEQ15" s="1"/>
+      <c r="AER15" s="1"/>
+      <c r="AES15" s="1"/>
+      <c r="AET15" s="1"/>
+      <c r="AEU15" s="1"/>
+      <c r="AEV15" s="1"/>
+      <c r="AEW15" s="1"/>
+      <c r="AEX15" s="1"/>
+      <c r="AEY15" s="1"/>
+      <c r="AEZ15" s="1"/>
+      <c r="AFA15" s="1"/>
+      <c r="AFB15" s="1"/>
+      <c r="AFC15" s="1"/>
+      <c r="AFD15" s="1"/>
+      <c r="AFE15" s="1"/>
+      <c r="AFF15" s="1"/>
+      <c r="AFG15" s="1"/>
+      <c r="AFH15" s="1"/>
+      <c r="AFI15" s="1"/>
+      <c r="AFJ15" s="1"/>
+      <c r="AFK15" s="1"/>
+      <c r="AFL15" s="1"/>
+      <c r="AFM15" s="1"/>
+      <c r="AFN15" s="1"/>
+      <c r="AFO15" s="1"/>
+      <c r="AFP15" s="1"/>
+      <c r="AFQ15" s="1"/>
+      <c r="AFR15" s="1"/>
+      <c r="AFS15" s="1"/>
+      <c r="AFT15" s="1"/>
+      <c r="AFU15" s="1"/>
+      <c r="AFV15" s="1"/>
+      <c r="AFW15" s="1"/>
+      <c r="AFX15" s="1"/>
+      <c r="AFY15" s="1"/>
+      <c r="AFZ15" s="1"/>
+      <c r="AGA15" s="1"/>
+      <c r="AGB15" s="1"/>
+      <c r="AGC15" s="1"/>
+      <c r="AGD15" s="1"/>
+      <c r="AGE15" s="1"/>
+      <c r="AGF15" s="1"/>
+      <c r="AGG15" s="1"/>
+      <c r="AGH15" s="1"/>
+      <c r="AGI15" s="1"/>
+      <c r="AGJ15" s="1"/>
+      <c r="AGK15" s="1"/>
+      <c r="AGL15" s="1"/>
+      <c r="AGM15" s="1"/>
+      <c r="AGN15" s="1"/>
+      <c r="AGO15" s="1"/>
+      <c r="AGP15" s="1"/>
+      <c r="AGQ15" s="1"/>
+      <c r="AGR15" s="1"/>
+      <c r="AGS15" s="1"/>
+      <c r="AGT15" s="1"/>
+      <c r="AGU15" s="1"/>
+      <c r="AGV15" s="1"/>
+      <c r="AGW15" s="1"/>
+      <c r="AGX15" s="1"/>
+      <c r="AGY15" s="1"/>
+      <c r="AGZ15" s="1"/>
+      <c r="AHA15" s="1"/>
+      <c r="AHB15" s="1"/>
+      <c r="AHC15" s="1"/>
+      <c r="AHD15" s="1"/>
+      <c r="AHE15" s="1"/>
+      <c r="AHF15" s="1"/>
+      <c r="AHG15" s="1"/>
+      <c r="AHH15" s="1"/>
+      <c r="AHI15" s="1"/>
+      <c r="AHJ15" s="1"/>
+      <c r="AHK15" s="1"/>
+      <c r="AHL15" s="1"/>
+      <c r="AHM15" s="1"/>
+      <c r="AHN15" s="1"/>
+      <c r="AHO15" s="1"/>
+      <c r="AHP15" s="1"/>
+      <c r="AHQ15" s="1"/>
+      <c r="AHR15" s="1"/>
+      <c r="AHS15" s="1"/>
+      <c r="AHT15" s="1"/>
+      <c r="AHU15" s="1"/>
+      <c r="AHV15" s="1"/>
+      <c r="AHW15" s="1"/>
+      <c r="AHX15" s="1"/>
+      <c r="AHY15" s="1"/>
+      <c r="AHZ15" s="1"/>
+      <c r="AIA15" s="1"/>
+      <c r="AIB15" s="1"/>
+      <c r="AIC15" s="1"/>
+      <c r="AID15" s="1"/>
+      <c r="AIE15" s="1"/>
+      <c r="AIF15" s="1"/>
+      <c r="AIG15" s="1"/>
+      <c r="AIH15" s="1"/>
+      <c r="AII15" s="1"/>
+      <c r="AIJ15" s="1"/>
+      <c r="AIK15" s="1"/>
+      <c r="AIL15" s="1"/>
+      <c r="AIM15" s="1"/>
+      <c r="AIN15" s="1"/>
+      <c r="AIO15" s="1"/>
+      <c r="AIP15" s="1"/>
+      <c r="AIQ15" s="1"/>
+      <c r="AIR15" s="1"/>
+      <c r="AIS15" s="1"/>
+      <c r="AIT15" s="1"/>
+      <c r="AIU15" s="1"/>
+      <c r="AIV15" s="1"/>
+      <c r="AIW15" s="1"/>
+      <c r="AIX15" s="1"/>
+      <c r="AIY15" s="1"/>
+      <c r="AIZ15" s="1"/>
+      <c r="AJA15" s="1"/>
+      <c r="AJB15" s="1"/>
+      <c r="AJC15" s="1"/>
+      <c r="AJD15" s="1"/>
+      <c r="AJE15" s="1"/>
+      <c r="AJF15" s="1"/>
+      <c r="AJG15" s="1"/>
+      <c r="AJH15" s="1"/>
+      <c r="AJI15" s="1"/>
+      <c r="AJJ15" s="1"/>
+      <c r="AJK15" s="1"/>
+      <c r="AJL15" s="1"/>
+      <c r="AJM15" s="1"/>
+      <c r="AJN15" s="1"/>
+      <c r="AJO15" s="1"/>
+      <c r="AJP15" s="1"/>
+      <c r="AJQ15" s="1"/>
+      <c r="AJR15" s="1"/>
+      <c r="AJS15" s="1"/>
+      <c r="AJT15" s="1"/>
+      <c r="AJU15" s="1"/>
+      <c r="AJV15" s="1"/>
+      <c r="AJW15" s="1"/>
+      <c r="AJX15" s="1"/>
+      <c r="AJY15" s="1"/>
+      <c r="AJZ15" s="1"/>
+      <c r="AKA15" s="1"/>
+      <c r="AKB15" s="1"/>
+      <c r="AKC15" s="1"/>
+      <c r="AKD15" s="1"/>
+      <c r="AKE15" s="1"/>
+      <c r="AKF15" s="1"/>
+      <c r="AKG15" s="1"/>
+      <c r="AKH15" s="1"/>
+      <c r="AKI15" s="1"/>
+      <c r="AKJ15" s="1"/>
+      <c r="AKK15" s="1"/>
+      <c r="AKL15" s="1"/>
+      <c r="AKM15" s="1"/>
+      <c r="AKN15" s="1"/>
+      <c r="AKO15" s="1"/>
+      <c r="AKP15" s="1"/>
+      <c r="AKQ15" s="1"/>
+      <c r="AKR15" s="1"/>
+      <c r="AKS15" s="1"/>
+      <c r="AKT15" s="1"/>
+      <c r="AKU15" s="1"/>
+      <c r="AKV15" s="1"/>
+      <c r="AKW15" s="1"/>
+      <c r="AKX15" s="1"/>
+      <c r="AKY15" s="1"/>
+      <c r="AKZ15" s="1"/>
+      <c r="ALA15" s="1"/>
+      <c r="ALB15" s="1"/>
+      <c r="ALC15" s="1"/>
+      <c r="ALD15" s="1"/>
+      <c r="ALE15" s="1"/>
+      <c r="ALF15" s="1"/>
+      <c r="ALG15" s="1"/>
+      <c r="ALH15" s="1"/>
+      <c r="ALI15" s="1"/>
+      <c r="ALJ15" s="1"/>
+      <c r="ALK15" s="1"/>
+      <c r="ALL15" s="1"/>
+      <c r="ALM15" s="1"/>
+      <c r="ALN15" s="1"/>
+      <c r="ALO15" s="1"/>
+      <c r="ALP15" s="1"/>
+      <c r="ALQ15" s="1"/>
+      <c r="ALR15" s="1"/>
+      <c r="ALS15" s="1"/>
+      <c r="ALT15" s="1"/>
+      <c r="ALU15" s="1"/>
+      <c r="ALV15" s="1"/>
+      <c r="ALW15" s="1"/>
+      <c r="ALX15" s="1"/>
+      <c r="ALY15" s="1"/>
+      <c r="ALZ15" s="1"/>
+      <c r="AMA15" s="1"/>
+      <c r="AMB15" s="1"/>
+      <c r="AMC15" s="1"/>
+      <c r="AMD15" s="1"/>
+      <c r="AME15" s="1"/>
+      <c r="AMF15" s="1"/>
+      <c r="AMG15" s="1"/>
+      <c r="AMH15" s="1"/>
+      <c r="AMI15" s="1"/>
+      <c r="AMJ15" s="1"/>
+      <c r="AMK15" s="1"/>
+    </row>
+    <row r="28" ht="13.8" customHeight="1"/>
+    <row r="34" spans="8:1025" ht="13.2" customHeight="1">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="1"/>
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
+      <c r="AK34" s="1"/>
+      <c r="AL34" s="1"/>
+      <c r="AM34" s="1"/>
+      <c r="AN34" s="1"/>
+      <c r="AO34" s="1"/>
+      <c r="AP34" s="1"/>
+      <c r="AQ34" s="1"/>
+      <c r="AR34" s="1"/>
+      <c r="AS34" s="1"/>
+      <c r="AT34" s="1"/>
+      <c r="AU34" s="1"/>
+      <c r="AV34" s="1"/>
+      <c r="AW34" s="1"/>
+      <c r="AX34" s="1"/>
+      <c r="AY34" s="1"/>
+      <c r="AZ34" s="1"/>
+      <c r="BA34" s="1"/>
+      <c r="BB34" s="1"/>
+      <c r="BC34" s="1"/>
+      <c r="BD34" s="1"/>
+      <c r="BE34" s="1"/>
+      <c r="BF34" s="1"/>
+      <c r="BG34" s="1"/>
+      <c r="BH34" s="1"/>
+      <c r="BI34" s="1"/>
+      <c r="BJ34" s="1"/>
+      <c r="BK34" s="1"/>
+      <c r="BL34" s="1"/>
+      <c r="BM34" s="1"/>
+      <c r="BN34" s="1"/>
+      <c r="BO34" s="1"/>
+      <c r="BP34" s="1"/>
+      <c r="BQ34" s="1"/>
+      <c r="BR34" s="1"/>
+      <c r="BS34" s="1"/>
+      <c r="BT34" s="1"/>
+      <c r="BU34" s="1"/>
+      <c r="BV34" s="1"/>
+      <c r="BW34" s="1"/>
+      <c r="BX34" s="1"/>
+      <c r="BY34" s="1"/>
+      <c r="BZ34" s="1"/>
+      <c r="CA34" s="1"/>
+      <c r="CB34" s="1"/>
+      <c r="CC34" s="1"/>
+      <c r="CD34" s="1"/>
+      <c r="CE34" s="1"/>
+      <c r="CF34" s="1"/>
+      <c r="CG34" s="1"/>
+      <c r="CH34" s="1"/>
+      <c r="CI34" s="1"/>
+      <c r="CJ34" s="1"/>
+      <c r="CK34" s="1"/>
+      <c r="CL34" s="1"/>
+      <c r="CM34" s="1"/>
+      <c r="CN34" s="1"/>
+      <c r="CO34" s="1"/>
+      <c r="CP34" s="1"/>
+      <c r="CQ34" s="1"/>
+      <c r="CR34" s="1"/>
+      <c r="CS34" s="1"/>
+      <c r="CT34" s="1"/>
+      <c r="CU34" s="1"/>
+      <c r="CV34" s="1"/>
+      <c r="CW34" s="1"/>
+      <c r="CX34" s="1"/>
+      <c r="CY34" s="1"/>
+      <c r="CZ34" s="1"/>
+      <c r="DA34" s="1"/>
+      <c r="DB34" s="1"/>
+      <c r="DC34" s="1"/>
+      <c r="DD34" s="1"/>
+      <c r="DE34" s="1"/>
+      <c r="DF34" s="1"/>
+      <c r="DG34" s="1"/>
+      <c r="DH34" s="1"/>
+      <c r="DI34" s="1"/>
+      <c r="DJ34" s="1"/>
+      <c r="DK34" s="1"/>
+      <c r="DL34" s="1"/>
+      <c r="DM34" s="1"/>
+      <c r="DN34" s="1"/>
+      <c r="DO34" s="1"/>
+      <c r="DP34" s="1"/>
+      <c r="DQ34" s="1"/>
+      <c r="DR34" s="1"/>
+      <c r="DS34" s="1"/>
+      <c r="DT34" s="1"/>
+      <c r="DU34" s="1"/>
+      <c r="DV34" s="1"/>
+      <c r="DW34" s="1"/>
+      <c r="DX34" s="1"/>
+      <c r="DY34" s="1"/>
+      <c r="DZ34" s="1"/>
+      <c r="EA34" s="1"/>
+      <c r="EB34" s="1"/>
+      <c r="EC34" s="1"/>
+      <c r="ED34" s="1"/>
+      <c r="EE34" s="1"/>
+      <c r="EF34" s="1"/>
+      <c r="EG34" s="1"/>
+      <c r="EH34" s="1"/>
+      <c r="EI34" s="1"/>
+      <c r="EJ34" s="1"/>
+      <c r="EK34" s="1"/>
+      <c r="EL34" s="1"/>
+      <c r="EM34" s="1"/>
+      <c r="EN34" s="1"/>
+      <c r="EO34" s="1"/>
+      <c r="EP34" s="1"/>
+      <c r="EQ34" s="1"/>
+      <c r="ER34" s="1"/>
+      <c r="ES34" s="1"/>
+      <c r="ET34" s="1"/>
+      <c r="EU34" s="1"/>
+      <c r="EV34" s="1"/>
+      <c r="EW34" s="1"/>
+      <c r="EX34" s="1"/>
+      <c r="EY34" s="1"/>
+      <c r="EZ34" s="1"/>
+      <c r="FA34" s="1"/>
+      <c r="FB34" s="1"/>
+      <c r="FC34" s="1"/>
+      <c r="FD34" s="1"/>
+      <c r="FE34" s="1"/>
+      <c r="FF34" s="1"/>
+      <c r="FG34" s="1"/>
+      <c r="FH34" s="1"/>
+      <c r="FI34" s="1"/>
+      <c r="FJ34" s="1"/>
+      <c r="FK34" s="1"/>
+      <c r="FL34" s="1"/>
+      <c r="FM34" s="1"/>
+      <c r="FN34" s="1"/>
+      <c r="FO34" s="1"/>
+      <c r="FP34" s="1"/>
+      <c r="FQ34" s="1"/>
+      <c r="FR34" s="1"/>
+      <c r="FS34" s="1"/>
+      <c r="FT34" s="1"/>
+      <c r="FU34" s="1"/>
+      <c r="FV34" s="1"/>
+      <c r="FW34" s="1"/>
+      <c r="FX34" s="1"/>
+      <c r="FY34" s="1"/>
+      <c r="FZ34" s="1"/>
+      <c r="GA34" s="1"/>
+      <c r="GB34" s="1"/>
+      <c r="GC34" s="1"/>
+      <c r="GD34" s="1"/>
+      <c r="GE34" s="1"/>
+      <c r="GF34" s="1"/>
+      <c r="GG34" s="1"/>
+      <c r="GH34" s="1"/>
+      <c r="GI34" s="1"/>
+      <c r="GJ34" s="1"/>
+      <c r="GK34" s="1"/>
+      <c r="GL34" s="1"/>
+      <c r="GM34" s="1"/>
+      <c r="GN34" s="1"/>
+      <c r="GO34" s="1"/>
+      <c r="GP34" s="1"/>
+      <c r="GQ34" s="1"/>
+      <c r="GR34" s="1"/>
+      <c r="GS34" s="1"/>
+      <c r="GT34" s="1"/>
+      <c r="GU34" s="1"/>
+      <c r="GV34" s="1"/>
+      <c r="GW34" s="1"/>
+      <c r="GX34" s="1"/>
+      <c r="GY34" s="1"/>
+      <c r="GZ34" s="1"/>
+      <c r="HA34" s="1"/>
+      <c r="HB34" s="1"/>
+      <c r="HC34" s="1"/>
+      <c r="HD34" s="1"/>
+      <c r="HE34" s="1"/>
+      <c r="HF34" s="1"/>
+      <c r="HG34" s="1"/>
+      <c r="HH34" s="1"/>
+      <c r="HI34" s="1"/>
+      <c r="HJ34" s="1"/>
+      <c r="HK34" s="1"/>
+      <c r="HL34" s="1"/>
+      <c r="HM34" s="1"/>
+      <c r="HN34" s="1"/>
+      <c r="HO34" s="1"/>
+      <c r="HP34" s="1"/>
+      <c r="HQ34" s="1"/>
+      <c r="HR34" s="1"/>
+      <c r="HS34" s="1"/>
+      <c r="HT34" s="1"/>
+      <c r="HU34" s="1"/>
+      <c r="HV34" s="1"/>
+      <c r="HW34" s="1"/>
+      <c r="HX34" s="1"/>
+      <c r="HY34" s="1"/>
+      <c r="HZ34" s="1"/>
+      <c r="IA34" s="1"/>
+      <c r="IB34" s="1"/>
+      <c r="IC34" s="1"/>
+      <c r="ID34" s="1"/>
+      <c r="IE34" s="1"/>
+      <c r="IF34" s="1"/>
+      <c r="IG34" s="1"/>
+      <c r="IH34" s="1"/>
+      <c r="II34" s="1"/>
+      <c r="IJ34" s="1"/>
+      <c r="IK34" s="1"/>
+      <c r="IL34" s="1"/>
+      <c r="IM34" s="1"/>
+      <c r="IN34" s="1"/>
+      <c r="IO34" s="1"/>
+      <c r="IP34" s="1"/>
+      <c r="IQ34" s="1"/>
+      <c r="IR34" s="1"/>
+      <c r="IS34" s="1"/>
+      <c r="IT34" s="1"/>
+      <c r="IU34" s="1"/>
+      <c r="IV34" s="1"/>
+      <c r="IW34" s="1"/>
+      <c r="IX34" s="1"/>
+      <c r="IY34" s="1"/>
+      <c r="IZ34" s="1"/>
+      <c r="JA34" s="1"/>
+      <c r="JB34" s="1"/>
+      <c r="JC34" s="1"/>
+      <c r="JD34" s="1"/>
+      <c r="JE34" s="1"/>
+      <c r="JF34" s="1"/>
+      <c r="JG34" s="1"/>
+      <c r="JH34" s="1"/>
+      <c r="JI34" s="1"/>
+      <c r="JJ34" s="1"/>
+      <c r="JK34" s="1"/>
+      <c r="JL34" s="1"/>
+      <c r="JM34" s="1"/>
+      <c r="JN34" s="1"/>
+      <c r="JO34" s="1"/>
+      <c r="JP34" s="1"/>
+      <c r="JQ34" s="1"/>
+      <c r="JR34" s="1"/>
+      <c r="JS34" s="1"/>
+      <c r="JT34" s="1"/>
+      <c r="JU34" s="1"/>
+      <c r="JV34" s="1"/>
+      <c r="JW34" s="1"/>
+      <c r="JX34" s="1"/>
+      <c r="JY34" s="1"/>
+      <c r="JZ34" s="1"/>
+      <c r="KA34" s="1"/>
+      <c r="KB34" s="1"/>
+      <c r="KC34" s="1"/>
+      <c r="KD34" s="1"/>
+      <c r="KE34" s="1"/>
+      <c r="KF34" s="1"/>
+      <c r="KG34" s="1"/>
+      <c r="KH34" s="1"/>
+      <c r="KI34" s="1"/>
+      <c r="KJ34" s="1"/>
+      <c r="KK34" s="1"/>
+      <c r="KL34" s="1"/>
+      <c r="KM34" s="1"/>
+      <c r="KN34" s="1"/>
+      <c r="KO34" s="1"/>
+      <c r="KP34" s="1"/>
+      <c r="KQ34" s="1"/>
+      <c r="KR34" s="1"/>
+      <c r="KS34" s="1"/>
+      <c r="KT34" s="1"/>
+      <c r="KU34" s="1"/>
+      <c r="KV34" s="1"/>
+      <c r="KW34" s="1"/>
+      <c r="KX34" s="1"/>
+      <c r="KY34" s="1"/>
+      <c r="KZ34" s="1"/>
+      <c r="LA34" s="1"/>
+      <c r="LB34" s="1"/>
+      <c r="LC34" s="1"/>
+      <c r="LD34" s="1"/>
+      <c r="LE34" s="1"/>
+      <c r="LF34" s="1"/>
+      <c r="LG34" s="1"/>
+      <c r="LH34" s="1"/>
+      <c r="LI34" s="1"/>
+      <c r="LJ34" s="1"/>
+      <c r="LK34" s="1"/>
+      <c r="LL34" s="1"/>
+      <c r="LM34" s="1"/>
+      <c r="LN34" s="1"/>
+      <c r="LO34" s="1"/>
+      <c r="LP34" s="1"/>
+      <c r="LQ34" s="1"/>
+      <c r="LR34" s="1"/>
+      <c r="LS34" s="1"/>
+      <c r="LT34" s="1"/>
+      <c r="LU34" s="1"/>
+      <c r="LV34" s="1"/>
+      <c r="LW34" s="1"/>
+      <c r="LX34" s="1"/>
+      <c r="LY34" s="1"/>
+      <c r="LZ34" s="1"/>
+      <c r="MA34" s="1"/>
+      <c r="MB34" s="1"/>
+      <c r="MC34" s="1"/>
+      <c r="MD34" s="1"/>
+      <c r="ME34" s="1"/>
+      <c r="MF34" s="1"/>
+      <c r="MG34" s="1"/>
+      <c r="MH34" s="1"/>
+      <c r="MI34" s="1"/>
+      <c r="MJ34" s="1"/>
+      <c r="MK34" s="1"/>
+      <c r="ML34" s="1"/>
+      <c r="MM34" s="1"/>
+      <c r="MN34" s="1"/>
+      <c r="MO34" s="1"/>
+      <c r="MP34" s="1"/>
+      <c r="MQ34" s="1"/>
+      <c r="MR34" s="1"/>
+      <c r="MS34" s="1"/>
+      <c r="MT34" s="1"/>
+      <c r="MU34" s="1"/>
+      <c r="MV34" s="1"/>
+      <c r="MW34" s="1"/>
+      <c r="MX34" s="1"/>
+      <c r="MY34" s="1"/>
+      <c r="MZ34" s="1"/>
+      <c r="NA34" s="1"/>
+      <c r="NB34" s="1"/>
+      <c r="NC34" s="1"/>
+      <c r="ND34" s="1"/>
+      <c r="NE34" s="1"/>
+      <c r="NF34" s="1"/>
+      <c r="NG34" s="1"/>
+      <c r="NH34" s="1"/>
+      <c r="NI34" s="1"/>
+      <c r="NJ34" s="1"/>
+      <c r="NK34" s="1"/>
+      <c r="NL34" s="1"/>
+      <c r="NM34" s="1"/>
+      <c r="NN34" s="1"/>
+      <c r="NO34" s="1"/>
+      <c r="NP34" s="1"/>
+      <c r="NQ34" s="1"/>
+      <c r="NR34" s="1"/>
+      <c r="NS34" s="1"/>
+      <c r="NT34" s="1"/>
+      <c r="NU34" s="1"/>
+      <c r="NV34" s="1"/>
+      <c r="NW34" s="1"/>
+      <c r="NX34" s="1"/>
+      <c r="NY34" s="1"/>
+      <c r="NZ34" s="1"/>
+      <c r="OA34" s="1"/>
+      <c r="OB34" s="1"/>
+      <c r="OC34" s="1"/>
+      <c r="OD34" s="1"/>
+      <c r="OE34" s="1"/>
+      <c r="OF34" s="1"/>
+      <c r="OG34" s="1"/>
+      <c r="OH34" s="1"/>
+      <c r="OI34" s="1"/>
+      <c r="OJ34" s="1"/>
+      <c r="OK34" s="1"/>
+      <c r="OL34" s="1"/>
+      <c r="OM34" s="1"/>
+      <c r="ON34" s="1"/>
+      <c r="OO34" s="1"/>
+      <c r="OP34" s="1"/>
+      <c r="OQ34" s="1"/>
+      <c r="OR34" s="1"/>
+      <c r="OS34" s="1"/>
+      <c r="OT34" s="1"/>
+      <c r="OU34" s="1"/>
+      <c r="OV34" s="1"/>
+      <c r="OW34" s="1"/>
+      <c r="OX34" s="1"/>
+      <c r="OY34" s="1"/>
+      <c r="OZ34" s="1"/>
+      <c r="PA34" s="1"/>
+      <c r="PB34" s="1"/>
+      <c r="PC34" s="1"/>
+      <c r="PD34" s="1"/>
+      <c r="PE34" s="1"/>
+      <c r="PF34" s="1"/>
+      <c r="PG34" s="1"/>
+      <c r="PH34" s="1"/>
+      <c r="PI34" s="1"/>
+      <c r="PJ34" s="1"/>
+      <c r="PK34" s="1"/>
+      <c r="PL34" s="1"/>
+      <c r="PM34" s="1"/>
+      <c r="PN34" s="1"/>
+      <c r="PO34" s="1"/>
+      <c r="PP34" s="1"/>
+      <c r="PQ34" s="1"/>
+      <c r="PR34" s="1"/>
+      <c r="PS34" s="1"/>
+      <c r="PT34" s="1"/>
+      <c r="PU34" s="1"/>
+      <c r="PV34" s="1"/>
+      <c r="PW34" s="1"/>
+      <c r="PX34" s="1"/>
+      <c r="PY34" s="1"/>
+      <c r="PZ34" s="1"/>
+      <c r="QA34" s="1"/>
+      <c r="QB34" s="1"/>
+      <c r="QC34" s="1"/>
+      <c r="QD34" s="1"/>
+      <c r="QE34" s="1"/>
+      <c r="QF34" s="1"/>
+      <c r="QG34" s="1"/>
+      <c r="QH34" s="1"/>
+      <c r="QI34" s="1"/>
+      <c r="QJ34" s="1"/>
+      <c r="QK34" s="1"/>
+      <c r="QL34" s="1"/>
+      <c r="QM34" s="1"/>
+      <c r="QN34" s="1"/>
+      <c r="QO34" s="1"/>
+      <c r="QP34" s="1"/>
+      <c r="QQ34" s="1"/>
+      <c r="QR34" s="1"/>
+      <c r="QS34" s="1"/>
+      <c r="QT34" s="1"/>
+      <c r="QU34" s="1"/>
+      <c r="QV34" s="1"/>
+      <c r="QW34" s="1"/>
+      <c r="QX34" s="1"/>
+      <c r="QY34" s="1"/>
+      <c r="QZ34" s="1"/>
+      <c r="RA34" s="1"/>
+      <c r="RB34" s="1"/>
+      <c r="RC34" s="1"/>
+      <c r="RD34" s="1"/>
+      <c r="RE34" s="1"/>
+      <c r="RF34" s="1"/>
+      <c r="RG34" s="1"/>
+      <c r="RH34" s="1"/>
+      <c r="RI34" s="1"/>
+      <c r="RJ34" s="1"/>
+      <c r="RK34" s="1"/>
+      <c r="RL34" s="1"/>
+      <c r="RM34" s="1"/>
+      <c r="RN34" s="1"/>
+      <c r="RO34" s="1"/>
+      <c r="RP34" s="1"/>
+      <c r="RQ34" s="1"/>
+      <c r="RR34" s="1"/>
+      <c r="RS34" s="1"/>
+      <c r="RT34" s="1"/>
+      <c r="RU34" s="1"/>
+      <c r="RV34" s="1"/>
+      <c r="RW34" s="1"/>
+      <c r="RX34" s="1"/>
+      <c r="RY34" s="1"/>
+      <c r="RZ34" s="1"/>
+      <c r="SA34" s="1"/>
+      <c r="SB34" s="1"/>
+      <c r="SC34" s="1"/>
+      <c r="SD34" s="1"/>
+      <c r="SE34" s="1"/>
+      <c r="SF34" s="1"/>
+      <c r="SG34" s="1"/>
+      <c r="SH34" s="1"/>
+      <c r="SI34" s="1"/>
+      <c r="SJ34" s="1"/>
+      <c r="SK34" s="1"/>
+      <c r="SL34" s="1"/>
+      <c r="SM34" s="1"/>
+      <c r="SN34" s="1"/>
+      <c r="SO34" s="1"/>
+      <c r="SP34" s="1"/>
+      <c r="SQ34" s="1"/>
+      <c r="SR34" s="1"/>
+      <c r="SS34" s="1"/>
+      <c r="ST34" s="1"/>
+      <c r="SU34" s="1"/>
+      <c r="SV34" s="1"/>
+      <c r="SW34" s="1"/>
+      <c r="SX34" s="1"/>
+      <c r="SY34" s="1"/>
+      <c r="SZ34" s="1"/>
+      <c r="TA34" s="1"/>
+      <c r="TB34" s="1"/>
+      <c r="TC34" s="1"/>
+      <c r="TD34" s="1"/>
+      <c r="TE34" s="1"/>
+      <c r="TF34" s="1"/>
+      <c r="TG34" s="1"/>
+      <c r="TH34" s="1"/>
+      <c r="TI34" s="1"/>
+      <c r="TJ34" s="1"/>
+      <c r="TK34" s="1"/>
+      <c r="TL34" s="1"/>
+      <c r="TM34" s="1"/>
+      <c r="TN34" s="1"/>
+      <c r="TO34" s="1"/>
+      <c r="TP34" s="1"/>
+      <c r="TQ34" s="1"/>
+      <c r="TR34" s="1"/>
+      <c r="TS34" s="1"/>
+      <c r="TT34" s="1"/>
+      <c r="TU34" s="1"/>
+      <c r="TV34" s="1"/>
+      <c r="TW34" s="1"/>
+      <c r="TX34" s="1"/>
+      <c r="TY34" s="1"/>
+      <c r="TZ34" s="1"/>
+      <c r="UA34" s="1"/>
+      <c r="UB34" s="1"/>
+      <c r="UC34" s="1"/>
+      <c r="UD34" s="1"/>
+      <c r="UE34" s="1"/>
+      <c r="UF34" s="1"/>
+      <c r="UG34" s="1"/>
+      <c r="UH34" s="1"/>
+      <c r="UI34" s="1"/>
+      <c r="UJ34" s="1"/>
+      <c r="UK34" s="1"/>
+      <c r="UL34" s="1"/>
+      <c r="UM34" s="1"/>
+      <c r="UN34" s="1"/>
+      <c r="UO34" s="1"/>
+      <c r="UP34" s="1"/>
+      <c r="UQ34" s="1"/>
+      <c r="UR34" s="1"/>
+      <c r="US34" s="1"/>
+      <c r="UT34" s="1"/>
+      <c r="UU34" s="1"/>
+      <c r="UV34" s="1"/>
+      <c r="UW34" s="1"/>
+      <c r="UX34" s="1"/>
+      <c r="UY34" s="1"/>
+      <c r="UZ34" s="1"/>
+      <c r="VA34" s="1"/>
+      <c r="VB34" s="1"/>
+      <c r="VC34" s="1"/>
+      <c r="VD34" s="1"/>
+      <c r="VE34" s="1"/>
+      <c r="VF34" s="1"/>
+      <c r="VG34" s="1"/>
+      <c r="VH34" s="1"/>
+      <c r="VI34" s="1"/>
+      <c r="VJ34" s="1"/>
+      <c r="VK34" s="1"/>
+      <c r="VL34" s="1"/>
+      <c r="VM34" s="1"/>
+      <c r="VN34" s="1"/>
+      <c r="VO34" s="1"/>
+      <c r="VP34" s="1"/>
+      <c r="VQ34" s="1"/>
+      <c r="VR34" s="1"/>
+      <c r="VS34" s="1"/>
+      <c r="VT34" s="1"/>
+      <c r="VU34" s="1"/>
+      <c r="VV34" s="1"/>
+      <c r="VW34" s="1"/>
+      <c r="VX34" s="1"/>
+      <c r="VY34" s="1"/>
+      <c r="VZ34" s="1"/>
+      <c r="WA34" s="1"/>
+      <c r="WB34" s="1"/>
+      <c r="WC34" s="1"/>
+      <c r="WD34" s="1"/>
+      <c r="WE34" s="1"/>
+      <c r="WF34" s="1"/>
+      <c r="WG34" s="1"/>
+      <c r="WH34" s="1"/>
+      <c r="WI34" s="1"/>
+      <c r="WJ34" s="1"/>
+      <c r="WK34" s="1"/>
+      <c r="WL34" s="1"/>
+      <c r="WM34" s="1"/>
+      <c r="WN34" s="1"/>
+      <c r="WO34" s="1"/>
+      <c r="WP34" s="1"/>
+      <c r="WQ34" s="1"/>
+      <c r="WR34" s="1"/>
+      <c r="WS34" s="1"/>
+      <c r="WT34" s="1"/>
+      <c r="WU34" s="1"/>
+      <c r="WV34" s="1"/>
+      <c r="WW34" s="1"/>
+      <c r="WX34" s="1"/>
+      <c r="WY34" s="1"/>
+      <c r="WZ34" s="1"/>
+      <c r="XA34" s="1"/>
+      <c r="XB34" s="1"/>
+      <c r="XC34" s="1"/>
+      <c r="XD34" s="1"/>
+      <c r="XE34" s="1"/>
+      <c r="XF34" s="1"/>
+      <c r="XG34" s="1"/>
+      <c r="XH34" s="1"/>
+      <c r="XI34" s="1"/>
+      <c r="XJ34" s="1"/>
+      <c r="XK34" s="1"/>
+      <c r="XL34" s="1"/>
+      <c r="XM34" s="1"/>
+      <c r="XN34" s="1"/>
+      <c r="XO34" s="1"/>
+      <c r="XP34" s="1"/>
+      <c r="XQ34" s="1"/>
+      <c r="XR34" s="1"/>
+      <c r="XS34" s="1"/>
+      <c r="XT34" s="1"/>
+      <c r="XU34" s="1"/>
+      <c r="XV34" s="1"/>
+      <c r="XW34" s="1"/>
+      <c r="XX34" s="1"/>
+      <c r="XY34" s="1"/>
+      <c r="XZ34" s="1"/>
+      <c r="YA34" s="1"/>
+      <c r="YB34" s="1"/>
+      <c r="YC34" s="1"/>
+      <c r="YD34" s="1"/>
+      <c r="YE34" s="1"/>
+      <c r="YF34" s="1"/>
+      <c r="YG34" s="1"/>
+      <c r="YH34" s="1"/>
+      <c r="YI34" s="1"/>
+      <c r="YJ34" s="1"/>
+      <c r="YK34" s="1"/>
+      <c r="YL34" s="1"/>
+      <c r="YM34" s="1"/>
+      <c r="YN34" s="1"/>
+      <c r="YO34" s="1"/>
+      <c r="YP34" s="1"/>
+      <c r="YQ34" s="1"/>
+      <c r="YR34" s="1"/>
+      <c r="YS34" s="1"/>
+      <c r="YT34" s="1"/>
+      <c r="YU34" s="1"/>
+      <c r="YV34" s="1"/>
+      <c r="YW34" s="1"/>
+      <c r="YX34" s="1"/>
+      <c r="YY34" s="1"/>
+      <c r="YZ34" s="1"/>
+      <c r="ZA34" s="1"/>
+      <c r="ZB34" s="1"/>
+      <c r="ZC34" s="1"/>
+      <c r="ZD34" s="1"/>
+      <c r="ZE34" s="1"/>
+      <c r="ZF34" s="1"/>
+      <c r="ZG34" s="1"/>
+      <c r="ZH34" s="1"/>
+      <c r="ZI34" s="1"/>
+      <c r="ZJ34" s="1"/>
+      <c r="ZK34" s="1"/>
+      <c r="ZL34" s="1"/>
+      <c r="ZM34" s="1"/>
+      <c r="ZN34" s="1"/>
+      <c r="ZO34" s="1"/>
+      <c r="ZP34" s="1"/>
+      <c r="ZQ34" s="1"/>
+      <c r="ZR34" s="1"/>
+      <c r="ZS34" s="1"/>
+      <c r="ZT34" s="1"/>
+      <c r="ZU34" s="1"/>
+      <c r="ZV34" s="1"/>
+      <c r="ZW34" s="1"/>
+      <c r="ZX34" s="1"/>
+      <c r="ZY34" s="1"/>
+      <c r="ZZ34" s="1"/>
+      <c r="AAA34" s="1"/>
+      <c r="AAB34" s="1"/>
+      <c r="AAC34" s="1"/>
+      <c r="AAD34" s="1"/>
+      <c r="AAE34" s="1"/>
+      <c r="AAF34" s="1"/>
+      <c r="AAG34" s="1"/>
+      <c r="AAH34" s="1"/>
+      <c r="AAI34" s="1"/>
+      <c r="AAJ34" s="1"/>
+      <c r="AAK34" s="1"/>
+      <c r="AAL34" s="1"/>
+      <c r="AAM34" s="1"/>
+      <c r="AAN34" s="1"/>
+      <c r="AAO34" s="1"/>
+      <c r="AAP34" s="1"/>
+      <c r="AAQ34" s="1"/>
+      <c r="AAR34" s="1"/>
+      <c r="AAS34" s="1"/>
+      <c r="AAT34" s="1"/>
+      <c r="AAU34" s="1"/>
+      <c r="AAV34" s="1"/>
+      <c r="AAW34" s="1"/>
+      <c r="AAX34" s="1"/>
+      <c r="AAY34" s="1"/>
+      <c r="AAZ34" s="1"/>
+      <c r="ABA34" s="1"/>
+      <c r="ABB34" s="1"/>
+      <c r="ABC34" s="1"/>
+      <c r="ABD34" s="1"/>
+      <c r="ABE34" s="1"/>
+      <c r="ABF34" s="1"/>
+      <c r="ABG34" s="1"/>
+      <c r="ABH34" s="1"/>
+      <c r="ABI34" s="1"/>
+      <c r="ABJ34" s="1"/>
+      <c r="ABK34" s="1"/>
+      <c r="ABL34" s="1"/>
+      <c r="ABM34" s="1"/>
+      <c r="ABN34" s="1"/>
+      <c r="ABO34" s="1"/>
+      <c r="ABP34" s="1"/>
+      <c r="ABQ34" s="1"/>
+      <c r="ABR34" s="1"/>
+      <c r="ABS34" s="1"/>
+      <c r="ABT34" s="1"/>
+      <c r="ABU34" s="1"/>
+      <c r="ABV34" s="1"/>
+      <c r="ABW34" s="1"/>
+      <c r="ABX34" s="1"/>
+      <c r="ABY34" s="1"/>
+      <c r="ABZ34" s="1"/>
+      <c r="ACA34" s="1"/>
+      <c r="ACB34" s="1"/>
+      <c r="ACC34" s="1"/>
+      <c r="ACD34" s="1"/>
+      <c r="ACE34" s="1"/>
+      <c r="ACF34" s="1"/>
+      <c r="ACG34" s="1"/>
+      <c r="ACH34" s="1"/>
+      <c r="ACI34" s="1"/>
+      <c r="ACJ34" s="1"/>
+      <c r="ACK34" s="1"/>
+      <c r="ACL34" s="1"/>
+      <c r="ACM34" s="1"/>
+      <c r="ACN34" s="1"/>
+      <c r="ACO34" s="1"/>
+      <c r="ACP34" s="1"/>
+      <c r="ACQ34" s="1"/>
+      <c r="ACR34" s="1"/>
+      <c r="ACS34" s="1"/>
+      <c r="ACT34" s="1"/>
+      <c r="ACU34" s="1"/>
+      <c r="ACV34" s="1"/>
+      <c r="ACW34" s="1"/>
+      <c r="ACX34" s="1"/>
+      <c r="ACY34" s="1"/>
+      <c r="ACZ34" s="1"/>
+      <c r="ADA34" s="1"/>
+      <c r="ADB34" s="1"/>
+      <c r="ADC34" s="1"/>
+      <c r="ADD34" s="1"/>
+      <c r="ADE34" s="1"/>
+      <c r="ADF34" s="1"/>
+      <c r="ADG34" s="1"/>
+      <c r="ADH34" s="1"/>
+      <c r="ADI34" s="1"/>
+      <c r="ADJ34" s="1"/>
+      <c r="ADK34" s="1"/>
+      <c r="ADL34" s="1"/>
+      <c r="ADM34" s="1"/>
+      <c r="ADN34" s="1"/>
+      <c r="ADO34" s="1"/>
+      <c r="ADP34" s="1"/>
+      <c r="ADQ34" s="1"/>
+      <c r="ADR34" s="1"/>
+      <c r="ADS34" s="1"/>
+      <c r="ADT34" s="1"/>
+      <c r="ADU34" s="1"/>
+      <c r="ADV34" s="1"/>
+      <c r="ADW34" s="1"/>
+      <c r="ADX34" s="1"/>
+      <c r="ADY34" s="1"/>
+      <c r="ADZ34" s="1"/>
+      <c r="AEA34" s="1"/>
+      <c r="AEB34" s="1"/>
+      <c r="AEC34" s="1"/>
+      <c r="AED34" s="1"/>
+      <c r="AEE34" s="1"/>
+      <c r="AEF34" s="1"/>
+      <c r="AEG34" s="1"/>
+      <c r="AEH34" s="1"/>
+      <c r="AEI34" s="1"/>
+      <c r="AEJ34" s="1"/>
+      <c r="AEK34" s="1"/>
+      <c r="AEL34" s="1"/>
+      <c r="AEM34" s="1"/>
+      <c r="AEN34" s="1"/>
+      <c r="AEO34" s="1"/>
+      <c r="AEP34" s="1"/>
+      <c r="AEQ34" s="1"/>
+      <c r="AER34" s="1"/>
+      <c r="AES34" s="1"/>
+      <c r="AET34" s="1"/>
+      <c r="AEU34" s="1"/>
+      <c r="AEV34" s="1"/>
+      <c r="AEW34" s="1"/>
+      <c r="AEX34" s="1"/>
+      <c r="AEY34" s="1"/>
+      <c r="AEZ34" s="1"/>
+      <c r="AFA34" s="1"/>
+      <c r="AFB34" s="1"/>
+      <c r="AFC34" s="1"/>
+      <c r="AFD34" s="1"/>
+      <c r="AFE34" s="1"/>
+      <c r="AFF34" s="1"/>
+      <c r="AFG34" s="1"/>
+      <c r="AFH34" s="1"/>
+      <c r="AFI34" s="1"/>
+      <c r="AFJ34" s="1"/>
+      <c r="AFK34" s="1"/>
+      <c r="AFL34" s="1"/>
+      <c r="AFM34" s="1"/>
+      <c r="AFN34" s="1"/>
+      <c r="AFO34" s="1"/>
+      <c r="AFP34" s="1"/>
+      <c r="AFQ34" s="1"/>
+      <c r="AFR34" s="1"/>
+      <c r="AFS34" s="1"/>
+      <c r="AFT34" s="1"/>
+      <c r="AFU34" s="1"/>
+      <c r="AFV34" s="1"/>
+      <c r="AFW34" s="1"/>
+      <c r="AFX34" s="1"/>
+      <c r="AFY34" s="1"/>
+      <c r="AFZ34" s="1"/>
+      <c r="AGA34" s="1"/>
+      <c r="AGB34" s="1"/>
+      <c r="AGC34" s="1"/>
+      <c r="AGD34" s="1"/>
+      <c r="AGE34" s="1"/>
+      <c r="AGF34" s="1"/>
+      <c r="AGG34" s="1"/>
+      <c r="AGH34" s="1"/>
+      <c r="AGI34" s="1"/>
+      <c r="AGJ34" s="1"/>
+      <c r="AGK34" s="1"/>
+      <c r="AGL34" s="1"/>
+      <c r="AGM34" s="1"/>
+      <c r="AGN34" s="1"/>
+      <c r="AGO34" s="1"/>
+      <c r="AGP34" s="1"/>
+      <c r="AGQ34" s="1"/>
+      <c r="AGR34" s="1"/>
+      <c r="AGS34" s="1"/>
+      <c r="AGT34" s="1"/>
+      <c r="AGU34" s="1"/>
+      <c r="AGV34" s="1"/>
+      <c r="AGW34" s="1"/>
+      <c r="AGX34" s="1"/>
+      <c r="AGY34" s="1"/>
+      <c r="AGZ34" s="1"/>
+      <c r="AHA34" s="1"/>
+      <c r="AHB34" s="1"/>
+      <c r="AHC34" s="1"/>
+      <c r="AHD34" s="1"/>
+      <c r="AHE34" s="1"/>
+      <c r="AHF34" s="1"/>
+      <c r="AHG34" s="1"/>
+      <c r="AHH34" s="1"/>
+      <c r="AHI34" s="1"/>
+      <c r="AHJ34" s="1"/>
+      <c r="AHK34" s="1"/>
+      <c r="AHL34" s="1"/>
+      <c r="AHM34" s="1"/>
+      <c r="AHN34" s="1"/>
+      <c r="AHO34" s="1"/>
+      <c r="AHP34" s="1"/>
+      <c r="AHQ34" s="1"/>
+      <c r="AHR34" s="1"/>
+      <c r="AHS34" s="1"/>
+      <c r="AHT34" s="1"/>
+      <c r="AHU34" s="1"/>
+      <c r="AHV34" s="1"/>
+      <c r="AHW34" s="1"/>
+      <c r="AHX34" s="1"/>
+      <c r="AHY34" s="1"/>
+      <c r="AHZ34" s="1"/>
+      <c r="AIA34" s="1"/>
+      <c r="AIB34" s="1"/>
+      <c r="AIC34" s="1"/>
+      <c r="AID34" s="1"/>
+      <c r="AIE34" s="1"/>
+      <c r="AIF34" s="1"/>
+      <c r="AIG34" s="1"/>
+      <c r="AIH34" s="1"/>
+      <c r="AII34" s="1"/>
+      <c r="AIJ34" s="1"/>
+      <c r="AIK34" s="1"/>
+      <c r="AIL34" s="1"/>
+      <c r="AIM34" s="1"/>
+      <c r="AIN34" s="1"/>
+      <c r="AIO34" s="1"/>
+      <c r="AIP34" s="1"/>
+      <c r="AIQ34" s="1"/>
+      <c r="AIR34" s="1"/>
+      <c r="AIS34" s="1"/>
+      <c r="AIT34" s="1"/>
+      <c r="AIU34" s="1"/>
+      <c r="AIV34" s="1"/>
+      <c r="AIW34" s="1"/>
+      <c r="AIX34" s="1"/>
+      <c r="AIY34" s="1"/>
+      <c r="AIZ34" s="1"/>
+      <c r="AJA34" s="1"/>
+      <c r="AJB34" s="1"/>
+      <c r="AJC34" s="1"/>
+      <c r="AJD34" s="1"/>
+      <c r="AJE34" s="1"/>
+      <c r="AJF34" s="1"/>
+      <c r="AJG34" s="1"/>
+      <c r="AJH34" s="1"/>
+      <c r="AJI34" s="1"/>
+      <c r="AJJ34" s="1"/>
+      <c r="AJK34" s="1"/>
+      <c r="AJL34" s="1"/>
+      <c r="AJM34" s="1"/>
+      <c r="AJN34" s="1"/>
+      <c r="AJO34" s="1"/>
+      <c r="AJP34" s="1"/>
+      <c r="AJQ34" s="1"/>
+      <c r="AJR34" s="1"/>
+      <c r="AJS34" s="1"/>
+      <c r="AJT34" s="1"/>
+      <c r="AJU34" s="1"/>
+      <c r="AJV34" s="1"/>
+      <c r="AJW34" s="1"/>
+      <c r="AJX34" s="1"/>
+      <c r="AJY34" s="1"/>
+      <c r="AJZ34" s="1"/>
+      <c r="AKA34" s="1"/>
+      <c r="AKB34" s="1"/>
+      <c r="AKC34" s="1"/>
+      <c r="AKD34" s="1"/>
+      <c r="AKE34" s="1"/>
+      <c r="AKF34" s="1"/>
+      <c r="AKG34" s="1"/>
+      <c r="AKH34" s="1"/>
+      <c r="AKI34" s="1"/>
+      <c r="AKJ34" s="1"/>
+      <c r="AKK34" s="1"/>
+      <c r="AKL34" s="1"/>
+      <c r="AKM34" s="1"/>
+      <c r="AKN34" s="1"/>
+      <c r="AKO34" s="1"/>
+      <c r="AKP34" s="1"/>
+      <c r="AKQ34" s="1"/>
+      <c r="AKR34" s="1"/>
+      <c r="AKS34" s="1"/>
+      <c r="AKT34" s="1"/>
+      <c r="AKU34" s="1"/>
+      <c r="AKV34" s="1"/>
+      <c r="AKW34" s="1"/>
+      <c r="AKX34" s="1"/>
+      <c r="AKY34" s="1"/>
+      <c r="AKZ34" s="1"/>
+      <c r="ALA34" s="1"/>
+      <c r="ALB34" s="1"/>
+      <c r="ALC34" s="1"/>
+      <c r="ALD34" s="1"/>
+      <c r="ALE34" s="1"/>
+      <c r="ALF34" s="1"/>
+      <c r="ALG34" s="1"/>
+      <c r="ALH34" s="1"/>
+      <c r="ALI34" s="1"/>
+      <c r="ALJ34" s="1"/>
+      <c r="ALK34" s="1"/>
+      <c r="ALL34" s="1"/>
+      <c r="ALM34" s="1"/>
+      <c r="ALN34" s="1"/>
+      <c r="ALO34" s="1"/>
+      <c r="ALP34" s="1"/>
+      <c r="ALQ34" s="1"/>
+      <c r="ALR34" s="1"/>
+      <c r="ALS34" s="1"/>
+      <c r="ALT34" s="1"/>
+      <c r="ALU34" s="1"/>
+      <c r="ALV34" s="1"/>
+      <c r="ALW34" s="1"/>
+      <c r="ALX34" s="1"/>
+      <c r="ALY34" s="1"/>
+      <c r="ALZ34" s="1"/>
+      <c r="AMA34" s="1"/>
+      <c r="AMB34" s="1"/>
+      <c r="AMC34" s="1"/>
+      <c r="AMD34" s="1"/>
+      <c r="AME34" s="1"/>
+      <c r="AMF34" s="1"/>
+      <c r="AMG34" s="1"/>
+      <c r="AMH34" s="1"/>
+      <c r="AMI34" s="1"/>
+      <c r="AMJ34" s="1"/>
+      <c r="AMK34" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D19945-73CE-4993-B520-52D08F9F6172}">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="12"/>
+    <col min="2" max="7" width="0" style="12" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="13">
+        <f>SUM(G3:G9)</f>
+        <v>46</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="13">
+        <f>AVERAGE(G3:G9)</f>
+        <v>6.5714285714285712</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:G9" si="0">SUM(B3:F3)</f>
+        <v>4</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>8</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>8</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="14">
+        <f>SUM(G12:G18)</f>
+        <v>48</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="14">
+        <f>AVERAGE(G12:G18)</f>
+        <v>6.8571428571428568</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" ref="G12:G18" si="1">SUM(B12:F12)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>8</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" s="14">
+        <f>SUM(G22:G28)</f>
+        <v>46</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" s="14">
+        <f>AVERAGE(G22:G28)</f>
+        <v>6.5714285714285712</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" ref="G22:G28" si="2">SUM(B22:F22)</f>
+        <v>5</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>8</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>8</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0</v>
+      </c>
+      <c r="C25" s="9">
+        <v>8</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>5</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I29" s="14">
+        <f>SUM(G30:G36)</f>
+        <v>48</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K29" s="14">
+        <f>AVERAGE(G30:G36)</f>
+        <v>6.8571428571428568</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>8</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" ref="G30:G36" si="3">SUM(B30:F30)</f>
+        <v>8</v>
+      </c>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9">
+        <v>5</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="1">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="9">
+        <v>4</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H34" s="14"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="9">
+        <v>0</v>
+      </c>
+      <c r="C35" s="9">
+        <v>8</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="9">
+        <v>0</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <v>8</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>